<commit_message>
validar un registro del excel, si existe, continuar al siguiente, caso contrario, guardar en db
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E5FA52-F0C7-4D78-B31A-DB4B10F48DD7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8D807-2793-4457-A14D-5A3AEFD02BD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>45264.45511574074</v>
+        <v>45264.496527777781</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45264.627800925926</v>
+        <v>45264.62777777778</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
paginación, reportes, cambio al registro de asistencia (se registraba una sola hora, ahora se le registra primera y segunda entrada y salida
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8D807-2793-4457-A14D-5A3AEFD02BD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6113BAA1-A221-4498-9A80-BF6341BC1E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVG231060035_attlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="1">
   <si>
     <t>a</t>
   </si>
@@ -569,9 +569,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +609,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -715,7 +715,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -865,24 +865,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F880"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>45264.496527777781</v>
+        <v>45111.33011574074</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -897,12 +897,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45264.62777777778</v>
+        <v>45111.54446759259</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -917,44 +917,3322 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45112.330474537041</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45112.544317129628</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45112.591249999998</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45112.733657407407</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45114.326597222222</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45114.563738425924</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45117.32671296296</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45117.545347222222</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45117.585497685184</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45117.7809375</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45118.327685185184</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45118.546666666669</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45118.587546296294</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45118.745439814818</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45119.328090277777</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45119.593657407408</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45119.757013888891</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45120.328923611109</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45103.659120370372</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45110.611990740741</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45110.640416666669</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45110.642326388886</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45111.322592592594</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45111.542199074072</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45111.583541666667</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45111.726631944446</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45112.327939814815</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45112.543252314812</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45112.580520833333</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45112.740486111114</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45114.332650462966</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45118.330567129633</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45118.54383101852</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45118.595486111109</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45118.765208333331</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45119.332083333335</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45119.542314814818</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45119.58222222222</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45119.77715277778</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45120.332627314812</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="1"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="1"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="1"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="1"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="1"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="1"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="1"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="1"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="1"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="1"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="1"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="1"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="1"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="1"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B192" s="1"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="1"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="1"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" s="1"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="1"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="1"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="1"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="1"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B203" s="1"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B204" s="1"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="1"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B206" s="1"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B207" s="1"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B208" s="1"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="1"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B210" s="1"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B211" s="1"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="1"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B213" s="1"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B214" s="1"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B215" s="1"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="1"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B217" s="1"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B218" s="1"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="1"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B220" s="1"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B221" s="1"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B222" s="1"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B223" s="1"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B224" s="1"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B225" s="1"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B226" s="1"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B227" s="1"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B228" s="1"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B229" s="1"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B230" s="1"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B231" s="1"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B232" s="1"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B233" s="1"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B234" s="1"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B235" s="1"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B236" s="1"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B237" s="1"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B238" s="1"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="1"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B240" s="1"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" s="1"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B242" s="1"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" s="1"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B244" s="1"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B245" s="1"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B246" s="1"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B247" s="1"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B248" s="1"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B249" s="1"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B250" s="1"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B251" s="1"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B252" s="1"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B253" s="1"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B254" s="1"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B255" s="1"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B256" s="1"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B257" s="1"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B258" s="1"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B259" s="1"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B260" s="1"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B261" s="1"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B262" s="1"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B263" s="1"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B264" s="1"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B265" s="1"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B266" s="1"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B267" s="1"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B268" s="1"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B269" s="1"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B270" s="1"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B271" s="1"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B272" s="1"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B273" s="1"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B274" s="1"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B275" s="1"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B276" s="1"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B277" s="1"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B278" s="1"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B279" s="1"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B280" s="1"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="1"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="1"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="1"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="1"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" s="1"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B286" s="1"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B287" s="1"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B288" s="1"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B289" s="1"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B290" s="1"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B291" s="1"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B292" s="1"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B293" s="1"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B294" s="1"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B295" s="1"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="1"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B297" s="1"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B298" s="1"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B299" s="1"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B300" s="1"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B301" s="1"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B302" s="1"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B303" s="1"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B304" s="1"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B305" s="1"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B306" s="1"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B307" s="1"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B308" s="1"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B309" s="1"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B310" s="1"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B311" s="1"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B312" s="1"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B313" s="1"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B314" s="1"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B315" s="1"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B316" s="1"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B317" s="1"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B318" s="1"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B319" s="1"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B320" s="1"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B321" s="1"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B322" s="1"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B323" s="1"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B324" s="1"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B325" s="1"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B326" s="1"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B327" s="1"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B328" s="1"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B329" s="1"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B330" s="1"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B331" s="1"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B332" s="1"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B333" s="1"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B334" s="1"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B335" s="1"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B336" s="1"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B337" s="1"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B338" s="1"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B339" s="1"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B340" s="1"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B341" s="1"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B342" s="1"/>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B343" s="1"/>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B344" s="1"/>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B345" s="1"/>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B346" s="1"/>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B347" s="1"/>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B348" s="1"/>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B349" s="1"/>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B350" s="1"/>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B351" s="1"/>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B352" s="1"/>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B353" s="1"/>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B354" s="1"/>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B355" s="1"/>
+    </row>
+    <row r="356" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B356" s="1"/>
+    </row>
+    <row r="357" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B357" s="1"/>
+    </row>
+    <row r="358" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B358" s="1"/>
+    </row>
+    <row r="359" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B359" s="1"/>
+    </row>
+    <row r="360" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B360" s="1"/>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B361" s="1"/>
+    </row>
+    <row r="362" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B362" s="1"/>
+    </row>
+    <row r="363" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B363" s="1"/>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B364" s="1"/>
+    </row>
+    <row r="365" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B365" s="1"/>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B366" s="1"/>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B367" s="1"/>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B368" s="1"/>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B369" s="1"/>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B370" s="1"/>
+    </row>
+    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B371" s="1"/>
+    </row>
+    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B372" s="1"/>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B373" s="1"/>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B374" s="1"/>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B375" s="1"/>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B376" s="1"/>
+    </row>
+    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B377" s="1"/>
+    </row>
+    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B378" s="1"/>
+    </row>
+    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B379" s="1"/>
+    </row>
+    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B380" s="1"/>
+    </row>
+    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B381" s="1"/>
+    </row>
+    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B382" s="1"/>
+    </row>
+    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B383" s="1"/>
+    </row>
+    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B384" s="1"/>
+    </row>
+    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B385" s="1"/>
+    </row>
+    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B386" s="1"/>
+    </row>
+    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B387" s="1"/>
+    </row>
+    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B388" s="1"/>
+    </row>
+    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B389" s="1"/>
+    </row>
+    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B390" s="1"/>
+    </row>
+    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B391" s="1"/>
+    </row>
+    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B392" s="1"/>
+    </row>
+    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B393" s="1"/>
+    </row>
+    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B394" s="1"/>
+    </row>
+    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B395" s="1"/>
+    </row>
+    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B396" s="1"/>
+    </row>
+    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B397" s="1"/>
+    </row>
+    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B398" s="1"/>
+    </row>
+    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B399" s="1"/>
+    </row>
+    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B400" s="1"/>
+    </row>
+    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B401" s="1"/>
+    </row>
+    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B402" s="1"/>
+    </row>
+    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B403" s="1"/>
+    </row>
+    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B404" s="1"/>
+    </row>
+    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B405" s="1"/>
+    </row>
+    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B406" s="1"/>
+    </row>
+    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B407" s="1"/>
+    </row>
+    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B408" s="1"/>
+    </row>
+    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B409" s="1"/>
+    </row>
+    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B410" s="1"/>
+    </row>
+    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B411" s="1"/>
+    </row>
+    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B412" s="1"/>
+    </row>
+    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B413" s="1"/>
+    </row>
+    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B414" s="1"/>
+    </row>
+    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B415" s="1"/>
+    </row>
+    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B416" s="1"/>
+    </row>
+    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B417" s="1"/>
+    </row>
+    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B418" s="1"/>
+    </row>
+    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B419" s="1"/>
+    </row>
+    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B420" s="1"/>
+    </row>
+    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B421" s="1"/>
+    </row>
+    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B422" s="1"/>
+    </row>
+    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B423" s="1"/>
+    </row>
+    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B424" s="1"/>
+    </row>
+    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B425" s="1"/>
+    </row>
+    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B426" s="1"/>
+    </row>
+    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B427" s="1"/>
+    </row>
+    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B428" s="1"/>
+    </row>
+    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B429" s="1"/>
+    </row>
+    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B430" s="1"/>
+    </row>
+    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B431" s="1"/>
+    </row>
+    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B432" s="1"/>
+    </row>
+    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B433" s="1"/>
+    </row>
+    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B434" s="1"/>
+    </row>
+    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B435" s="1"/>
+    </row>
+    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B436" s="1"/>
+    </row>
+    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B437" s="1"/>
+    </row>
+    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B438" s="1"/>
+    </row>
+    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B439" s="1"/>
+    </row>
+    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B440" s="1"/>
+    </row>
+    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B441" s="1"/>
+    </row>
+    <row r="442" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B442" s="1"/>
+    </row>
+    <row r="443" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B443" s="1"/>
+    </row>
+    <row r="444" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B444" s="1"/>
+    </row>
+    <row r="445" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B445" s="1"/>
+    </row>
+    <row r="446" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B446" s="1"/>
+    </row>
+    <row r="447" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B447" s="1"/>
+    </row>
+    <row r="448" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B448" s="1"/>
+    </row>
+    <row r="449" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B449" s="1"/>
+    </row>
+    <row r="450" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B450" s="1"/>
+    </row>
+    <row r="451" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B451" s="1"/>
+    </row>
+    <row r="452" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B452" s="1"/>
+    </row>
+    <row r="453" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B453" s="1"/>
+    </row>
+    <row r="454" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B454" s="1"/>
+    </row>
+    <row r="455" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B455" s="1"/>
+    </row>
+    <row r="456" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B456" s="1"/>
+    </row>
+    <row r="457" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B457" s="1"/>
+    </row>
+    <row r="458" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B458" s="1"/>
+    </row>
+    <row r="459" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B459" s="1"/>
+    </row>
+    <row r="460" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B460" s="1"/>
+    </row>
+    <row r="461" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B461" s="1"/>
+    </row>
+    <row r="462" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B462" s="1"/>
+    </row>
+    <row r="463" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B463" s="1"/>
+    </row>
+    <row r="464" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B464" s="1"/>
+    </row>
+    <row r="465" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B465" s="1"/>
+    </row>
+    <row r="466" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B466" s="1"/>
+    </row>
+    <row r="467" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B467" s="1"/>
+    </row>
+    <row r="468" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B468" s="1"/>
+    </row>
+    <row r="469" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B469" s="1"/>
+    </row>
+    <row r="470" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B470" s="1"/>
+    </row>
+    <row r="471" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B471" s="1"/>
+    </row>
+    <row r="472" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B472" s="1"/>
+    </row>
+    <row r="473" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B473" s="1"/>
+    </row>
+    <row r="474" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B474" s="1"/>
+    </row>
+    <row r="475" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B475" s="1"/>
+    </row>
+    <row r="476" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B476" s="1"/>
+    </row>
+    <row r="477" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B477" s="1"/>
+    </row>
+    <row r="478" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B478" s="1"/>
+    </row>
+    <row r="479" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B479" s="1"/>
+    </row>
+    <row r="480" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B480" s="1"/>
+    </row>
+    <row r="481" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B481" s="1"/>
+    </row>
+    <row r="482" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B482" s="1"/>
+    </row>
+    <row r="483" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B483" s="1"/>
+    </row>
+    <row r="484" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B484" s="1"/>
+    </row>
+    <row r="485" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B485" s="1"/>
+    </row>
+    <row r="486" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B486" s="1"/>
+    </row>
+    <row r="487" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B487" s="1"/>
+    </row>
+    <row r="488" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B488" s="1"/>
+    </row>
+    <row r="489" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B489" s="1"/>
+    </row>
+    <row r="490" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B490" s="1"/>
+    </row>
+    <row r="491" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B491" s="1"/>
+    </row>
+    <row r="492" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B492" s="1"/>
+    </row>
+    <row r="493" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B493" s="1"/>
+    </row>
+    <row r="494" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B494" s="1"/>
+    </row>
+    <row r="495" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B495" s="1"/>
+    </row>
+    <row r="496" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B496" s="1"/>
+    </row>
+    <row r="497" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B497" s="1"/>
+    </row>
+    <row r="498" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B498" s="1"/>
+    </row>
+    <row r="499" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B499" s="1"/>
+    </row>
+    <row r="500" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B500" s="1"/>
+    </row>
+    <row r="501" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B501" s="1"/>
+    </row>
+    <row r="502" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B502" s="1"/>
+    </row>
+    <row r="503" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B503" s="1"/>
+    </row>
+    <row r="504" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B504" s="1"/>
+    </row>
+    <row r="505" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B505" s="1"/>
+    </row>
+    <row r="506" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B506" s="1"/>
+    </row>
+    <row r="507" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B507" s="1"/>
+    </row>
+    <row r="508" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B508" s="1"/>
+    </row>
+    <row r="509" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B509" s="1"/>
+    </row>
+    <row r="510" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B510" s="1"/>
+    </row>
+    <row r="511" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B511" s="1"/>
+    </row>
+    <row r="512" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B512" s="1"/>
+    </row>
+    <row r="513" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B513" s="1"/>
+    </row>
+    <row r="514" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B514" s="1"/>
+    </row>
+    <row r="515" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B515" s="1"/>
+    </row>
+    <row r="516" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B516" s="1"/>
+    </row>
+    <row r="517" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B517" s="1"/>
+    </row>
+    <row r="518" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B518" s="1"/>
+    </row>
+    <row r="519" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B519" s="1"/>
+    </row>
+    <row r="520" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B520" s="1"/>
+    </row>
+    <row r="521" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B521" s="1"/>
+    </row>
+    <row r="522" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B522" s="1"/>
+    </row>
+    <row r="523" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B523" s="1"/>
+    </row>
+    <row r="524" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B524" s="1"/>
+    </row>
+    <row r="525" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B525" s="1"/>
+    </row>
+    <row r="526" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B526" s="1"/>
+    </row>
+    <row r="527" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B527" s="1"/>
+    </row>
+    <row r="528" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B528" s="1"/>
+    </row>
+    <row r="529" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B529" s="1"/>
+    </row>
+    <row r="530" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B530" s="1"/>
+    </row>
+    <row r="531" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B531" s="1"/>
+    </row>
+    <row r="532" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B532" s="1"/>
+    </row>
+    <row r="533" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B533" s="1"/>
+    </row>
+    <row r="534" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B534" s="1"/>
+    </row>
+    <row r="535" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B535" s="1"/>
+    </row>
+    <row r="536" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B536" s="1"/>
+    </row>
+    <row r="537" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B537" s="1"/>
+    </row>
+    <row r="538" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B538" s="1"/>
+    </row>
+    <row r="539" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B539" s="1"/>
+    </row>
+    <row r="540" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B540" s="1"/>
+    </row>
+    <row r="541" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B541" s="1"/>
+    </row>
+    <row r="542" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B542" s="1"/>
+    </row>
+    <row r="543" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B543" s="1"/>
+    </row>
+    <row r="544" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B544" s="1"/>
+    </row>
+    <row r="545" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B545" s="1"/>
+    </row>
+    <row r="546" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B546" s="1"/>
+    </row>
+    <row r="547" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B547" s="1"/>
+    </row>
+    <row r="548" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B548" s="1"/>
+    </row>
+    <row r="549" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B549" s="1"/>
+    </row>
+    <row r="550" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B550" s="1"/>
+    </row>
+    <row r="551" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B551" s="1"/>
+    </row>
+    <row r="552" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B552" s="1"/>
+    </row>
+    <row r="553" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B553" s="1"/>
+    </row>
+    <row r="554" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B554" s="1"/>
+    </row>
+    <row r="555" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B555" s="1"/>
+    </row>
+    <row r="556" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B556" s="1"/>
+    </row>
+    <row r="557" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B557" s="1"/>
+    </row>
+    <row r="558" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B558" s="1"/>
+    </row>
+    <row r="559" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B559" s="1"/>
+    </row>
+    <row r="560" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B560" s="1"/>
+    </row>
+    <row r="561" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B561" s="1"/>
+    </row>
+    <row r="562" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B562" s="1"/>
+    </row>
+    <row r="563" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B563" s="1"/>
+    </row>
+    <row r="564" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B564" s="1"/>
+    </row>
+    <row r="565" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B565" s="1"/>
+    </row>
+    <row r="566" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B566" s="1"/>
+    </row>
+    <row r="567" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B567" s="1"/>
+    </row>
+    <row r="568" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B568" s="1"/>
+    </row>
+    <row r="569" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B569" s="1"/>
+    </row>
+    <row r="570" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B570" s="1"/>
+    </row>
+    <row r="571" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B571" s="1"/>
+    </row>
+    <row r="572" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B572" s="1"/>
+    </row>
+    <row r="573" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B573" s="1"/>
+    </row>
+    <row r="574" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B574" s="1"/>
+    </row>
+    <row r="575" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B575" s="1"/>
+    </row>
+    <row r="576" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B576" s="1"/>
+    </row>
+    <row r="577" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B577" s="1"/>
+    </row>
+    <row r="578" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B578" s="1"/>
+    </row>
+    <row r="579" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B579" s="1"/>
+    </row>
+    <row r="580" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B580" s="1"/>
+    </row>
+    <row r="581" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B581" s="1"/>
+    </row>
+    <row r="582" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B582" s="1"/>
+    </row>
+    <row r="583" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B583" s="1"/>
+    </row>
+    <row r="584" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B584" s="1"/>
+    </row>
+    <row r="585" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B585" s="1"/>
+    </row>
+    <row r="586" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B586" s="1"/>
+    </row>
+    <row r="587" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B587" s="1"/>
+    </row>
+    <row r="588" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B588" s="1"/>
+    </row>
+    <row r="589" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B589" s="1"/>
+    </row>
+    <row r="590" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B590" s="1"/>
+    </row>
+    <row r="591" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B591" s="1"/>
+    </row>
+    <row r="592" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B592" s="1"/>
+    </row>
+    <row r="593" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B593" s="1"/>
+    </row>
+    <row r="594" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B594" s="1"/>
+    </row>
+    <row r="595" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B595" s="1"/>
+    </row>
+    <row r="596" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B596" s="1"/>
+    </row>
+    <row r="597" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B597" s="1"/>
+    </row>
+    <row r="598" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B598" s="1"/>
+    </row>
+    <row r="599" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B599" s="1"/>
+    </row>
+    <row r="600" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B600" s="1"/>
+    </row>
+    <row r="601" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B601" s="1"/>
+    </row>
+    <row r="602" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B602" s="1"/>
+    </row>
+    <row r="603" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B603" s="1"/>
+    </row>
+    <row r="604" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B604" s="1"/>
+    </row>
+    <row r="605" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B605" s="1"/>
+    </row>
+    <row r="606" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B606" s="1"/>
+    </row>
+    <row r="607" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B607" s="1"/>
+    </row>
+    <row r="608" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B608" s="1"/>
+    </row>
+    <row r="609" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B609" s="1"/>
+    </row>
+    <row r="610" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B610" s="1"/>
+    </row>
+    <row r="611" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B611" s="1"/>
+    </row>
+    <row r="612" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B612" s="1"/>
+    </row>
+    <row r="613" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B613" s="1"/>
+    </row>
+    <row r="614" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B614" s="1"/>
+    </row>
+    <row r="615" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B615" s="1"/>
+    </row>
+    <row r="616" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B616" s="1"/>
+    </row>
+    <row r="617" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B617" s="1"/>
+    </row>
+    <row r="618" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B618" s="1"/>
+    </row>
+    <row r="619" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B619" s="1"/>
+    </row>
+    <row r="620" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B620" s="1"/>
+    </row>
+    <row r="621" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B621" s="1"/>
+    </row>
+    <row r="622" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B622" s="1"/>
+    </row>
+    <row r="623" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B623" s="1"/>
+    </row>
+    <row r="624" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B624" s="1"/>
+    </row>
+    <row r="625" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B625" s="1"/>
+    </row>
+    <row r="626" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B626" s="1"/>
+    </row>
+    <row r="627" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B627" s="1"/>
+    </row>
+    <row r="628" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B628" s="1"/>
+    </row>
+    <row r="629" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B629" s="1"/>
+    </row>
+    <row r="630" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B630" s="1"/>
+    </row>
+    <row r="631" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B631" s="1"/>
+    </row>
+    <row r="632" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B632" s="1"/>
+    </row>
+    <row r="633" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B633" s="1"/>
+    </row>
+    <row r="634" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B634" s="1"/>
+    </row>
+    <row r="635" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B635" s="1"/>
+    </row>
+    <row r="636" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B636" s="1"/>
+    </row>
+    <row r="637" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B637" s="1"/>
+    </row>
+    <row r="638" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B638" s="1"/>
+    </row>
+    <row r="639" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B639" s="1"/>
+    </row>
+    <row r="640" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B640" s="1"/>
+    </row>
+    <row r="641" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B641" s="1"/>
+    </row>
+    <row r="642" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B642" s="1"/>
+    </row>
+    <row r="643" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B643" s="1"/>
+    </row>
+    <row r="644" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B644" s="1"/>
+    </row>
+    <row r="645" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B645" s="1"/>
+    </row>
+    <row r="646" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B646" s="1"/>
+    </row>
+    <row r="647" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B647" s="1"/>
+    </row>
+    <row r="648" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B648" s="1"/>
+    </row>
+    <row r="649" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B649" s="1"/>
+    </row>
+    <row r="650" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B650" s="1"/>
+    </row>
+    <row r="651" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B651" s="1"/>
+    </row>
+    <row r="652" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B652" s="1"/>
+    </row>
+    <row r="653" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B653" s="1"/>
+    </row>
+    <row r="654" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B654" s="1"/>
+    </row>
+    <row r="655" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B655" s="1"/>
+    </row>
+    <row r="656" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B656" s="1"/>
+    </row>
+    <row r="657" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B657" s="1"/>
+    </row>
+    <row r="658" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B658" s="1"/>
+    </row>
+    <row r="659" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B659" s="1"/>
+    </row>
+    <row r="660" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B660" s="1"/>
+    </row>
+    <row r="661" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B661" s="1"/>
+    </row>
+    <row r="662" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B662" s="1"/>
+    </row>
+    <row r="663" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B663" s="1"/>
+    </row>
+    <row r="664" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B664" s="1"/>
+    </row>
+    <row r="665" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B665" s="1"/>
+    </row>
+    <row r="666" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B666" s="1"/>
+    </row>
+    <row r="667" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B667" s="1"/>
+    </row>
+    <row r="668" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B668" s="1"/>
+    </row>
+    <row r="669" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B669" s="1"/>
+    </row>
+    <row r="670" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B670" s="1"/>
+    </row>
+    <row r="671" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B671" s="1"/>
+    </row>
+    <row r="672" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B672" s="1"/>
+    </row>
+    <row r="673" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B673" s="1"/>
+    </row>
+    <row r="674" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B674" s="1"/>
+    </row>
+    <row r="675" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B675" s="1"/>
+    </row>
+    <row r="676" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B676" s="1"/>
+    </row>
+    <row r="677" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B677" s="1"/>
+    </row>
+    <row r="678" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B678" s="1"/>
+    </row>
+    <row r="679" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B679" s="1"/>
+    </row>
+    <row r="680" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B680" s="1"/>
+    </row>
+    <row r="681" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B681" s="1"/>
+    </row>
+    <row r="682" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B682" s="1"/>
+    </row>
+    <row r="683" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B683" s="1"/>
+    </row>
+    <row r="684" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B684" s="1"/>
+    </row>
+    <row r="685" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B685" s="1"/>
+    </row>
+    <row r="686" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B686" s="1"/>
+    </row>
+    <row r="687" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B687" s="1"/>
+    </row>
+    <row r="688" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B688" s="1"/>
+    </row>
+    <row r="689" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B689" s="1"/>
+    </row>
+    <row r="690" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B690" s="1"/>
+    </row>
+    <row r="691" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B691" s="1"/>
+    </row>
+    <row r="692" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B692" s="1"/>
+    </row>
+    <row r="693" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B693" s="1"/>
+    </row>
+    <row r="694" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B694" s="1"/>
+    </row>
+    <row r="695" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B695" s="1"/>
+    </row>
+    <row r="696" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B696" s="1"/>
+    </row>
+    <row r="697" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B697" s="1"/>
+    </row>
+    <row r="698" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B698" s="1"/>
+    </row>
+    <row r="699" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B699" s="1"/>
+    </row>
+    <row r="700" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B700" s="1"/>
+    </row>
+    <row r="701" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B701" s="1"/>
+    </row>
+    <row r="702" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B702" s="1"/>
+    </row>
+    <row r="703" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B703" s="1"/>
+    </row>
+    <row r="704" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B704" s="1"/>
+    </row>
+    <row r="705" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B705" s="1"/>
+    </row>
+    <row r="706" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B706" s="1"/>
+    </row>
+    <row r="707" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B707" s="1"/>
+    </row>
+    <row r="708" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B708" s="1"/>
+    </row>
+    <row r="709" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B709" s="1"/>
+    </row>
+    <row r="710" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B710" s="1"/>
+    </row>
+    <row r="711" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B711" s="1"/>
+    </row>
+    <row r="712" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B712" s="1"/>
+    </row>
+    <row r="713" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B713" s="1"/>
+    </row>
+    <row r="714" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B714" s="1"/>
+    </row>
+    <row r="715" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B715" s="1"/>
+    </row>
+    <row r="716" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B716" s="1"/>
+    </row>
+    <row r="717" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B717" s="1"/>
+    </row>
+    <row r="718" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B718" s="1"/>
+    </row>
+    <row r="719" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B719" s="1"/>
+    </row>
+    <row r="720" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B720" s="1"/>
+    </row>
+    <row r="721" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B721" s="1"/>
+    </row>
+    <row r="722" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B722" s="1"/>
+    </row>
+    <row r="723" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B723" s="1"/>
+    </row>
+    <row r="724" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B724" s="1"/>
+    </row>
+    <row r="725" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B725" s="1"/>
+    </row>
+    <row r="726" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B726" s="1"/>
+    </row>
+    <row r="727" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B727" s="1"/>
+    </row>
+    <row r="728" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B728" s="1"/>
+    </row>
+    <row r="729" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B729" s="1"/>
+    </row>
+    <row r="730" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B730" s="1"/>
+    </row>
+    <row r="731" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B731" s="1"/>
+    </row>
+    <row r="732" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B732" s="1"/>
+    </row>
+    <row r="733" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B733" s="1"/>
+    </row>
+    <row r="734" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B734" s="1"/>
+    </row>
+    <row r="735" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B735" s="1"/>
+    </row>
+    <row r="736" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B736" s="1"/>
+    </row>
+    <row r="737" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B737" s="1"/>
+    </row>
+    <row r="738" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B738" s="1"/>
+    </row>
+    <row r="739" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B739" s="1"/>
+    </row>
+    <row r="740" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B740" s="1"/>
+    </row>
+    <row r="741" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B741" s="1"/>
+    </row>
+    <row r="742" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B742" s="1"/>
+    </row>
+    <row r="743" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B743" s="1"/>
+    </row>
+    <row r="744" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B744" s="1"/>
+    </row>
+    <row r="745" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B745" s="1"/>
+    </row>
+    <row r="746" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B746" s="1"/>
+    </row>
+    <row r="747" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B747" s="1"/>
+    </row>
+    <row r="748" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B748" s="1"/>
+    </row>
+    <row r="749" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B749" s="1"/>
+    </row>
+    <row r="750" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B750" s="1"/>
+    </row>
+    <row r="751" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B751" s="1"/>
+    </row>
+    <row r="752" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B752" s="1"/>
+    </row>
+    <row r="753" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B753" s="1"/>
+    </row>
+    <row r="754" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B754" s="1"/>
+    </row>
+    <row r="755" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B755" s="1"/>
+    </row>
+    <row r="756" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B756" s="1"/>
+    </row>
+    <row r="757" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B757" s="1"/>
+    </row>
+    <row r="758" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B758" s="1"/>
+    </row>
+    <row r="759" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B759" s="1"/>
+    </row>
+    <row r="760" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B760" s="1"/>
+    </row>
+    <row r="761" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B761" s="1"/>
+    </row>
+    <row r="762" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B762" s="1"/>
+    </row>
+    <row r="763" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B763" s="1"/>
+    </row>
+    <row r="764" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B764" s="1"/>
+    </row>
+    <row r="765" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B765" s="1"/>
+    </row>
+    <row r="766" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B766" s="1"/>
+    </row>
+    <row r="767" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B767" s="1"/>
+    </row>
+    <row r="768" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B768" s="1"/>
+    </row>
+    <row r="769" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B769" s="1"/>
+    </row>
+    <row r="770" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B770" s="1"/>
+    </row>
+    <row r="771" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B771" s="1"/>
+    </row>
+    <row r="772" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B772" s="1"/>
+    </row>
+    <row r="773" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B773" s="1"/>
+    </row>
+    <row r="774" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B774" s="1"/>
+    </row>
+    <row r="775" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B775" s="1"/>
+    </row>
+    <row r="776" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B776" s="1"/>
+    </row>
+    <row r="777" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B777" s="1"/>
+    </row>
+    <row r="778" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B778" s="1"/>
+    </row>
+    <row r="779" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B779" s="1"/>
+    </row>
+    <row r="780" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B780" s="1"/>
+    </row>
+    <row r="781" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B781" s="1"/>
+    </row>
+    <row r="782" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B782" s="1"/>
+    </row>
+    <row r="783" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B783" s="1"/>
+    </row>
+    <row r="784" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B784" s="1"/>
+    </row>
+    <row r="785" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B785" s="1"/>
+    </row>
+    <row r="786" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B786" s="1"/>
+    </row>
+    <row r="787" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B787" s="1"/>
+    </row>
+    <row r="788" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B788" s="1"/>
+    </row>
+    <row r="789" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B789" s="1"/>
+    </row>
+    <row r="790" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B790" s="1"/>
+    </row>
+    <row r="791" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B791" s="1"/>
+    </row>
+    <row r="792" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B792" s="1"/>
+    </row>
+    <row r="793" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B793" s="1"/>
+    </row>
+    <row r="794" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B794" s="1"/>
+    </row>
+    <row r="795" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B795" s="1"/>
+    </row>
+    <row r="796" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B796" s="1"/>
+    </row>
+    <row r="797" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B797" s="1"/>
+    </row>
+    <row r="798" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B798" s="1"/>
+    </row>
+    <row r="799" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B799" s="1"/>
+    </row>
+    <row r="800" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B800" s="1"/>
+    </row>
+    <row r="801" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B801" s="1"/>
+    </row>
+    <row r="802" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B802" s="1"/>
+    </row>
+    <row r="803" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B803" s="1"/>
+    </row>
+    <row r="804" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B804" s="1"/>
+    </row>
+    <row r="805" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B805" s="1"/>
+    </row>
+    <row r="806" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B806" s="1"/>
+    </row>
+    <row r="807" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B807" s="1"/>
+    </row>
+    <row r="808" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B808" s="1"/>
+    </row>
+    <row r="809" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B809" s="1"/>
+    </row>
+    <row r="810" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B810" s="1"/>
+    </row>
+    <row r="811" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B811" s="1"/>
+    </row>
+    <row r="812" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B812" s="1"/>
+    </row>
+    <row r="813" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B813" s="1"/>
+    </row>
+    <row r="814" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B814" s="1"/>
+    </row>
+    <row r="815" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B815" s="1"/>
+    </row>
+    <row r="816" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B816" s="1"/>
+    </row>
+    <row r="817" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B817" s="1"/>
+    </row>
+    <row r="818" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B818" s="1"/>
+    </row>
+    <row r="819" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B819" s="1"/>
+    </row>
+    <row r="820" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B820" s="1"/>
+    </row>
+    <row r="821" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B821" s="1"/>
+    </row>
+    <row r="822" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B822" s="1"/>
+    </row>
+    <row r="823" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B823" s="1"/>
+    </row>
+    <row r="824" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B824" s="1"/>
+    </row>
+    <row r="825" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B825" s="1"/>
+    </row>
+    <row r="826" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B826" s="1"/>
+    </row>
+    <row r="827" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B827" s="1"/>
+    </row>
+    <row r="828" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B828" s="1"/>
+    </row>
+    <row r="829" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B829" s="1"/>
+    </row>
+    <row r="830" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B830" s="1"/>
+    </row>
+    <row r="831" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B831" s="1"/>
+    </row>
+    <row r="832" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B832" s="1"/>
+    </row>
+    <row r="833" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B833" s="1"/>
+    </row>
+    <row r="834" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B834" s="1"/>
+    </row>
+    <row r="835" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B835" s="1"/>
+    </row>
+    <row r="836" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B836" s="1"/>
+    </row>
+    <row r="837" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B837" s="1"/>
+    </row>
+    <row r="838" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B838" s="1"/>
+    </row>
+    <row r="839" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B839" s="1"/>
+    </row>
+    <row r="840" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B840" s="1"/>
+    </row>
+    <row r="841" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B841" s="1"/>
+    </row>
+    <row r="842" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B842" s="1"/>
+    </row>
+    <row r="843" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B843" s="1"/>
+    </row>
+    <row r="844" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B844" s="1"/>
+    </row>
+    <row r="845" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B845" s="1"/>
+    </row>
+    <row r="846" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B846" s="1"/>
+    </row>
+    <row r="847" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B847" s="1"/>
+    </row>
+    <row r="848" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B848" s="1"/>
+    </row>
+    <row r="849" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B849" s="1"/>
+    </row>
+    <row r="850" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B850" s="1"/>
+    </row>
+    <row r="851" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B851" s="1"/>
+    </row>
+    <row r="852" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B852" s="1"/>
+    </row>
+    <row r="853" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B853" s="1"/>
+    </row>
+    <row r="854" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B854" s="1"/>
+    </row>
+    <row r="855" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B855" s="1"/>
+    </row>
+    <row r="856" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B856" s="1"/>
+    </row>
+    <row r="857" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B857" s="1"/>
+    </row>
+    <row r="858" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B858" s="1"/>
+    </row>
+    <row r="859" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B859" s="1"/>
+    </row>
+    <row r="860" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B860" s="1"/>
+    </row>
+    <row r="861" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B861" s="1"/>
+    </row>
+    <row r="862" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B862" s="1"/>
+    </row>
+    <row r="863" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B863" s="1"/>
+    </row>
+    <row r="864" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B864" s="1"/>
+    </row>
+    <row r="865" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B865" s="1"/>
+    </row>
+    <row r="866" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B866" s="1"/>
+    </row>
+    <row r="867" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B867" s="1"/>
+    </row>
+    <row r="868" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B868" s="1"/>
+    </row>
+    <row r="869" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B869" s="1"/>
+    </row>
+    <row r="870" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B870" s="1"/>
+    </row>
+    <row r="871" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B871" s="1"/>
+    </row>
+    <row r="872" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B872" s="1"/>
+    </row>
+    <row r="873" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B873" s="1"/>
+    </row>
+    <row r="874" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B874" s="1"/>
+    </row>
+    <row r="875" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B875" s="1"/>
+    </row>
+    <row r="876" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B876" s="1"/>
+    </row>
+    <row r="877" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B877" s="1"/>
+    </row>
+    <row r="878" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B878" s="1"/>
+    </row>
+    <row r="879" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B879" s="1"/>
+    </row>
+    <row r="880" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B880" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A1:F14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F882">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
filtros y nueva paginacion para el registro de asistencia y avance de filtros en los reportes
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6113BAA1-A221-4498-9A80-BF6341BC1E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61776037-745C-41EE-96F8-3AD078A3271B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVG231060035_attlog" sheetId="1" r:id="rId1"/>
@@ -569,9 +569,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +609,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -715,7 +715,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -867,22 +867,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>45111.33011574074</v>
+        <v>45728.33011574074</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -897,12 +897,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45111.54446759259</v>
+        <v>45728.54446759259</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -917,12 +917,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>45112.330474537041</v>
+        <v>45729.330474537041</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -937,12 +937,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>45112.544317129628</v>
+        <v>45729.544317129628</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -957,12 +957,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>45112.591249999998</v>
+        <v>45729.591249999998</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -977,12 +977,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>45112.733657407407</v>
+        <v>45729.733657407407</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -997,12 +997,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>45114.326597222222</v>
+        <v>45730.326597222222</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1017,12 +1017,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>45114.563738425924</v>
+        <v>45730.563738425924</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1037,12 +1037,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>45117.32671296296</v>
+        <v>45731.32671296296</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -1057,12 +1057,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>45117.545347222222</v>
+        <v>45731.545347222222</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -1077,12 +1077,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>45117.585497685184</v>
+        <v>45731.585497685184</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
@@ -1097,12 +1097,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <v>45117.7809375</v>
+        <v>45731.7809375</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -1117,12 +1117,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>45118.327685185184</v>
+        <v>45732.327685185184</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -1137,12 +1137,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>45118.546666666669</v>
+        <v>45732.546666666669</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
@@ -1157,12 +1157,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>45118.587546296294</v>
+        <v>45732.587546296294</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
@@ -1177,12 +1177,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>45118.745439814818</v>
+        <v>45732.745439814818</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
@@ -1197,12 +1197,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" s="1">
-        <v>45119.328090277777</v>
+        <v>45733.328090277777</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
@@ -1217,12 +1217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>45119.593657407408</v>
+        <v>45733.593657407408</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
@@ -1237,12 +1237,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="1">
-        <v>45119.757013888891</v>
+        <v>45733.757013888891</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
@@ -1257,12 +1257,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" s="1">
-        <v>45120.328923611109</v>
+        <v>45734.328923611109</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>0</v>
@@ -1277,12 +1277,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" s="1">
-        <v>45103.659120370372</v>
+        <v>45728.33011574074</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>0</v>
@@ -1297,12 +1297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>45110.611990740741</v>
+        <v>45728.54446759259</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>0</v>
@@ -1317,12 +1317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" s="1">
-        <v>45110.640416666669</v>
+        <v>45729.330474537041</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>0</v>
@@ -1334,15 +1334,15 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>45110.642326388886</v>
+        <v>45729.544317129628</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>0</v>
@@ -1357,12 +1357,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" s="1">
-        <v>45111.322592592594</v>
+        <v>45729.591249999998</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>0</v>
@@ -1377,12 +1377,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>45111.542199074072</v>
+        <v>45729.733657407407</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>0</v>
@@ -1397,12 +1397,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>45111.583541666667</v>
+        <v>45730.326597222222</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>0</v>
@@ -1417,12 +1417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>45111.726631944446</v>
+        <v>45730.563738425924</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>0</v>
@@ -1437,12 +1437,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29" s="1">
-        <v>45112.327939814815</v>
+        <v>45731.32671296296</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>0</v>
@@ -1457,12 +1457,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" s="1">
-        <v>45112.543252314812</v>
+        <v>45731.545347222222</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>0</v>
@@ -1477,12 +1477,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31" s="1">
-        <v>45112.580520833333</v>
+        <v>45731.585497685184</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>0</v>
@@ -1497,12 +1497,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32" s="1">
-        <v>45112.740486111114</v>
+        <v>45731.7809375</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>0</v>
@@ -1517,12 +1517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" s="1">
-        <v>45114.332650462966</v>
+        <v>45732.327685185184</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>0</v>
@@ -1537,12 +1537,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" s="1">
-        <v>45118.330567129633</v>
+        <v>45732.546666666669</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>0</v>
@@ -1557,12 +1557,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" s="1">
-        <v>45118.54383101852</v>
+        <v>45732.587546296294</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>0</v>
@@ -1577,12 +1577,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36" s="1">
-        <v>45118.595486111109</v>
+        <v>45732.745439814818</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>0</v>
@@ -1597,12 +1597,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
       <c r="B37" s="1">
-        <v>45118.765208333331</v>
+        <v>45733.328090277777</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>0</v>
@@ -1617,12 +1617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38" s="1">
-        <v>45119.332083333335</v>
+        <v>45733.593657407408</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>0</v>
@@ -1637,12 +1637,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" s="1">
-        <v>45119.542314814818</v>
+        <v>45733.757013888891</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>0</v>
@@ -1657,12 +1657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
       <c r="B40" s="1">
-        <v>45119.58222222222</v>
+        <v>45734.328923611109</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>0</v>
@@ -1677,12 +1677,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" s="1">
-        <v>45119.77715277778</v>
+        <v>45734.578923611109</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>0</v>
@@ -1697,12 +1697,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" s="1">
-        <v>45120.332627314812</v>
+        <v>45734.74559027778</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>0</v>
@@ -1717,2522 +1717,2522 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="1"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="1"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="1"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="1"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="1"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="1"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="1"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="1"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="1"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="1"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="1"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="1"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="1"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="1"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="1"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="1"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="1"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="1"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="1"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="1"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="1"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="1"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="1"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" s="1"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B216" s="1"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B217" s="1"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" s="1"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" s="1"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225" s="1"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226" s="1"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" s="1"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231" s="1"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232" s="1"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237" s="1"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238" s="1"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" s="1"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" s="1"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" s="1"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" s="1"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" s="1"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" s="1"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" s="1"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" s="1"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" s="1"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" s="1"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" s="1"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" s="1"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" s="1"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" s="1"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" s="1"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258" s="1"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259" s="1"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" s="1"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261" s="1"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B262" s="1"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" s="1"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B264" s="1"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B265" s="1"/>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266" s="1"/>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B267" s="1"/>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B268" s="1"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272" s="1"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B273" s="1"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B275" s="1"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B276" s="1"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B277" s="1"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B278" s="1"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B279" s="1"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B280" s="1"/>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B281" s="1"/>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B282" s="1"/>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B283" s="1"/>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B284" s="1"/>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B285" s="1"/>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B286" s="1"/>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B287" s="1"/>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B288" s="1"/>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B289" s="1"/>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B290" s="1"/>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B295" s="1"/>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B296" s="1"/>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B297" s="1"/>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B298" s="1"/>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B299" s="1"/>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B300" s="1"/>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B301" s="1"/>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B302" s="1"/>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B303" s="1"/>
     </row>
-    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B304" s="1"/>
     </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B305" s="1"/>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B306" s="1"/>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B307" s="1"/>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B308" s="1"/>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B309" s="1"/>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B310" s="1"/>
     </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B311" s="1"/>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B312" s="1"/>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B313" s="1"/>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B314" s="1"/>
     </row>
-    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B315" s="1"/>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B316" s="1"/>
     </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B317" s="1"/>
     </row>
-    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B318" s="1"/>
     </row>
-    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B319" s="1"/>
     </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B320" s="1"/>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B321" s="1"/>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B322" s="1"/>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B323" s="1"/>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B324" s="1"/>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B325" s="1"/>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" s="1"/>
     </row>
-    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B327" s="1"/>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B328" s="1"/>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B329" s="1"/>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B330" s="1"/>
     </row>
-    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B331" s="1"/>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B332" s="1"/>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B333" s="1"/>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B334" s="1"/>
     </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B335" s="1"/>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B336" s="1"/>
     </row>
-    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B337" s="1"/>
     </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B338" s="1"/>
     </row>
-    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B339" s="1"/>
     </row>
-    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="340" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B340" s="1"/>
     </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B341" s="1"/>
     </row>
-    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B342" s="1"/>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B343" s="1"/>
     </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B344" s="1"/>
     </row>
-    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B345" s="1"/>
     </row>
-    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B346" s="1"/>
     </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B347" s="1"/>
     </row>
-    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B348" s="1"/>
     </row>
-    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B349" s="1"/>
     </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B350" s="1"/>
     </row>
-    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="351" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B351" s="1"/>
     </row>
-    <row r="352" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="352" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B352" s="1"/>
     </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B353" s="1"/>
     </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B354" s="1"/>
     </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B355" s="1"/>
     </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B356" s="1"/>
     </row>
-    <row r="357" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B357" s="1"/>
     </row>
-    <row r="358" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B358" s="1"/>
     </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B359" s="1"/>
     </row>
-    <row r="360" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B360" s="1"/>
     </row>
-    <row r="361" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B361" s="1"/>
     </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B362" s="1"/>
     </row>
-    <row r="363" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B363" s="1"/>
     </row>
-    <row r="364" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B364" s="1"/>
     </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B365" s="1"/>
     </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B366" s="1"/>
     </row>
-    <row r="367" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B367" s="1"/>
     </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B368" s="1"/>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B369" s="1"/>
     </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B370" s="1"/>
     </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B371" s="1"/>
     </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B372" s="1"/>
     </row>
-    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B373" s="1"/>
     </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B374" s="1"/>
     </row>
-    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B375" s="1"/>
     </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B376" s="1"/>
     </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B377" s="1"/>
     </row>
-    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B378" s="1"/>
     </row>
-    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B379" s="1"/>
     </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B380" s="1"/>
     </row>
-    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B381" s="1"/>
     </row>
-    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B382" s="1"/>
     </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B383" s="1"/>
     </row>
-    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B384" s="1"/>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="385" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B385" s="1"/>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B386" s="1"/>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="387" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B387" s="1"/>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="388" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B388" s="1"/>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B389" s="1"/>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="390" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B390" s="1"/>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="391" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B391" s="1"/>
     </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B392" s="1"/>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="393" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B393" s="1"/>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="394" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B394" s="1"/>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B395" s="1"/>
     </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="396" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B396" s="1"/>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="397" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B397" s="1"/>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B398" s="1"/>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B399" s="1"/>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="400" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B400" s="1"/>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B401" s="1"/>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="402" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B402" s="1"/>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="403" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B403" s="1"/>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B404" s="1"/>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="405" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B405" s="1"/>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="406" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B406" s="1"/>
     </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="407" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B407" s="1"/>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="408" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B408" s="1"/>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="409" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B409" s="1"/>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B410" s="1"/>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="411" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B411" s="1"/>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="412" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B412" s="1"/>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B413" s="1"/>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="414" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B414" s="1"/>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="415" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B415" s="1"/>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B416" s="1"/>
     </row>
-    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="417" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B417" s="1"/>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="418" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B418" s="1"/>
     </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B419" s="1"/>
     </row>
-    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="420" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B420" s="1"/>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="421" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B421" s="1"/>
     </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B422" s="1"/>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="423" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B423" s="1"/>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="424" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B424" s="1"/>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B425" s="1"/>
     </row>
-    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="426" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B426" s="1"/>
     </row>
-    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="427" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B427" s="1"/>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B428" s="1"/>
     </row>
-    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="429" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B429" s="1"/>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="430" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B430" s="1"/>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="431" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B431" s="1"/>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="432" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B432" s="1"/>
     </row>
-    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="433" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B433" s="1"/>
     </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B434" s="1"/>
     </row>
-    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="435" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B435" s="1"/>
     </row>
-    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="436" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B436" s="1"/>
     </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B437" s="1"/>
     </row>
-    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="438" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B438" s="1"/>
     </row>
-    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="439" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B439" s="1"/>
     </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B440" s="1"/>
     </row>
-    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="441" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B441" s="1"/>
     </row>
-    <row r="442" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="442" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B442" s="1"/>
     </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B443" s="1"/>
     </row>
-    <row r="444" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="444" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B444" s="1"/>
     </row>
-    <row r="445" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="445" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B445" s="1"/>
     </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B446" s="1"/>
     </row>
-    <row r="447" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="447" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B447" s="1"/>
     </row>
-    <row r="448" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="448" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B448" s="1"/>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" s="1"/>
     </row>
-    <row r="450" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="450" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B450" s="1"/>
     </row>
-    <row r="451" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="451" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B451" s="1"/>
     </row>
-    <row r="452" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="452" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B452" s="1"/>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="453" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B453" s="1"/>
     </row>
-    <row r="454" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="454" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B454" s="1"/>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="455" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B455" s="1"/>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="456" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B456" s="1"/>
     </row>
-    <row r="457" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="457" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B457" s="1"/>
     </row>
-    <row r="458" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="458" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B458" s="1"/>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="459" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B459" s="1"/>
     </row>
-    <row r="460" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="460" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B460" s="1"/>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="461" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B461" s="1"/>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="462" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B462" s="1"/>
     </row>
-    <row r="463" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="463" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B463" s="1"/>
     </row>
-    <row r="464" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="464" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B464" s="1"/>
     </row>
-    <row r="465" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="465" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B465" s="1"/>
     </row>
-    <row r="466" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="466" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B466" s="1"/>
     </row>
-    <row r="467" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="467" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B467" s="1"/>
     </row>
-    <row r="468" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="468" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B468" s="1"/>
     </row>
-    <row r="469" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="469" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B469" s="1"/>
     </row>
-    <row r="470" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="470" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B470" s="1"/>
     </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="471" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B471" s="1"/>
     </row>
-    <row r="472" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="472" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B472" s="1"/>
     </row>
-    <row r="473" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="473" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B473" s="1"/>
     </row>
-    <row r="474" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="474" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B474" s="1"/>
     </row>
-    <row r="475" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="475" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B475" s="1"/>
     </row>
-    <row r="476" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="476" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B476" s="1"/>
     </row>
-    <row r="477" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="477" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B477" s="1"/>
     </row>
-    <row r="478" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="478" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B478" s="1"/>
     </row>
-    <row r="479" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="479" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B479" s="1"/>
     </row>
-    <row r="480" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="480" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B480" s="1"/>
     </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="481" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B481" s="1"/>
     </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="482" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B482" s="1"/>
     </row>
-    <row r="483" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="483" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B483" s="1"/>
     </row>
-    <row r="484" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="484" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B484" s="1"/>
     </row>
-    <row r="485" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="485" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B485" s="1"/>
     </row>
-    <row r="486" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="486" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B486" s="1"/>
     </row>
-    <row r="487" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="487" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B487" s="1"/>
     </row>
-    <row r="488" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="488" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B488" s="1"/>
     </row>
-    <row r="489" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="489" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B489" s="1"/>
     </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="490" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B490" s="1"/>
     </row>
-    <row r="491" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="491" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B491" s="1"/>
     </row>
-    <row r="492" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="492" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B492" s="1"/>
     </row>
-    <row r="493" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="493" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B493" s="1"/>
     </row>
-    <row r="494" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="494" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B494" s="1"/>
     </row>
-    <row r="495" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="495" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B495" s="1"/>
     </row>
-    <row r="496" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="496" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B496" s="1"/>
     </row>
-    <row r="497" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="497" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B497" s="1"/>
     </row>
-    <row r="498" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="498" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B498" s="1"/>
     </row>
-    <row r="499" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="499" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B499" s="1"/>
     </row>
-    <row r="500" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="500" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B500" s="1"/>
     </row>
-    <row r="501" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="501" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B501" s="1"/>
     </row>
-    <row r="502" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="502" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B502" s="1"/>
     </row>
-    <row r="503" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="503" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B503" s="1"/>
     </row>
-    <row r="504" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="504" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B504" s="1"/>
     </row>
-    <row r="505" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="505" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B505" s="1"/>
     </row>
-    <row r="506" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="506" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B506" s="1"/>
     </row>
-    <row r="507" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="507" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B507" s="1"/>
     </row>
-    <row r="508" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="508" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B508" s="1"/>
     </row>
-    <row r="509" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="509" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B509" s="1"/>
     </row>
-    <row r="510" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="510" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B510" s="1"/>
     </row>
-    <row r="511" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="511" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B511" s="1"/>
     </row>
-    <row r="512" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="512" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B512" s="1"/>
     </row>
-    <row r="513" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="513" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B513" s="1"/>
     </row>
-    <row r="514" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="514" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B514" s="1"/>
     </row>
-    <row r="515" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="515" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B515" s="1"/>
     </row>
-    <row r="516" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="516" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B516" s="1"/>
     </row>
-    <row r="517" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="517" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B517" s="1"/>
     </row>
-    <row r="518" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="518" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B518" s="1"/>
     </row>
-    <row r="519" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="519" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B519" s="1"/>
     </row>
-    <row r="520" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="520" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B520" s="1"/>
     </row>
-    <row r="521" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="521" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B521" s="1"/>
     </row>
-    <row r="522" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="522" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B522" s="1"/>
     </row>
-    <row r="523" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="523" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B523" s="1"/>
     </row>
-    <row r="524" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="524" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B524" s="1"/>
     </row>
-    <row r="525" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="525" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B525" s="1"/>
     </row>
-    <row r="526" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="526" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B526" s="1"/>
     </row>
-    <row r="527" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="527" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B527" s="1"/>
     </row>
-    <row r="528" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="528" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B528" s="1"/>
     </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="529" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B529" s="1"/>
     </row>
-    <row r="530" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="530" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B530" s="1"/>
     </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B531" s="1"/>
     </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="532" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B532" s="1"/>
     </row>
-    <row r="533" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="533" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B533" s="1"/>
     </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="534" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B534" s="1"/>
     </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="535" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B535" s="1"/>
     </row>
-    <row r="536" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="536" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B536" s="1"/>
     </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="537" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B537" s="1"/>
     </row>
-    <row r="538" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="538" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B538" s="1"/>
     </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="539" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B539" s="1"/>
     </row>
-    <row r="540" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="540" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B540" s="1"/>
     </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="541" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B541" s="1"/>
     </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="542" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B542" s="1"/>
     </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="543" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B543" s="1"/>
     </row>
-    <row r="544" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="544" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B544" s="1"/>
     </row>
-    <row r="545" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="545" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B545" s="1"/>
     </row>
-    <row r="546" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="546" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B546" s="1"/>
     </row>
-    <row r="547" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="547" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B547" s="1"/>
     </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="548" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B548" s="1"/>
     </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="549" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B549" s="1"/>
     </row>
-    <row r="550" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="550" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B550" s="1"/>
     </row>
-    <row r="551" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="551" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B551" s="1"/>
     </row>
-    <row r="552" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="552" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B552" s="1"/>
     </row>
-    <row r="553" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="553" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B553" s="1"/>
     </row>
-    <row r="554" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="554" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B554" s="1"/>
     </row>
-    <row r="555" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="555" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B555" s="1"/>
     </row>
-    <row r="556" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="556" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B556" s="1"/>
     </row>
-    <row r="557" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="557" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B557" s="1"/>
     </row>
-    <row r="558" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="558" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B558" s="1"/>
     </row>
-    <row r="559" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="559" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B559" s="1"/>
     </row>
-    <row r="560" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="560" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B560" s="1"/>
     </row>
-    <row r="561" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="561" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B561" s="1"/>
     </row>
-    <row r="562" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="562" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B562" s="1"/>
     </row>
-    <row r="563" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="563" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B563" s="1"/>
     </row>
-    <row r="564" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="564" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B564" s="1"/>
     </row>
-    <row r="565" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="565" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B565" s="1"/>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="566" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B566" s="1"/>
     </row>
-    <row r="567" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="567" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B567" s="1"/>
     </row>
-    <row r="568" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="568" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B568" s="1"/>
     </row>
-    <row r="569" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="569" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B569" s="1"/>
     </row>
-    <row r="570" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="570" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B570" s="1"/>
     </row>
-    <row r="571" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="571" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B571" s="1"/>
     </row>
-    <row r="572" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="572" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B572" s="1"/>
     </row>
-    <row r="573" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="573" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B573" s="1"/>
     </row>
-    <row r="574" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="574" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B574" s="1"/>
     </row>
-    <row r="575" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="575" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B575" s="1"/>
     </row>
-    <row r="576" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B576" s="1"/>
     </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="577" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B577" s="1"/>
     </row>
-    <row r="578" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="578" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B578" s="1"/>
     </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="579" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B579" s="1"/>
     </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="580" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B580" s="1"/>
     </row>
-    <row r="581" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="581" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B581" s="1"/>
     </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="582" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B582" s="1"/>
     </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="583" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B583" s="1"/>
     </row>
-    <row r="584" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="584" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B584" s="1"/>
     </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="585" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B585" s="1"/>
     </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="586" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B586" s="1"/>
     </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="587" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B587" s="1"/>
     </row>
-    <row r="588" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="588" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B588" s="1"/>
     </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="589" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B589" s="1"/>
     </row>
-    <row r="590" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="590" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B590" s="1"/>
     </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="591" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B591" s="1"/>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B592" s="1"/>
     </row>
-    <row r="593" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B593" s="1"/>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B594" s="1"/>
     </row>
-    <row r="595" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="595" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B595" s="1"/>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B596" s="1"/>
     </row>
-    <row r="597" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="597" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B597" s="1"/>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B598" s="1"/>
     </row>
-    <row r="599" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="599" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B599" s="1"/>
     </row>
-    <row r="600" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="600" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B600" s="1"/>
     </row>
-    <row r="601" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="601" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B601" s="1"/>
     </row>
-    <row r="602" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="602" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B602" s="1"/>
     </row>
-    <row r="603" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="603" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B603" s="1"/>
     </row>
-    <row r="604" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="604" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B604" s="1"/>
     </row>
-    <row r="605" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="605" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B605" s="1"/>
     </row>
-    <row r="606" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="606" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B606" s="1"/>
     </row>
-    <row r="607" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="607" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B607" s="1"/>
     </row>
-    <row r="608" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="608" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B608" s="1"/>
     </row>
-    <row r="609" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="609" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B609" s="1"/>
     </row>
-    <row r="610" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="610" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B610" s="1"/>
     </row>
-    <row r="611" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="611" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B611" s="1"/>
     </row>
-    <row r="612" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="612" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B612" s="1"/>
     </row>
-    <row r="613" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="613" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B613" s="1"/>
     </row>
-    <row r="614" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="614" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B614" s="1"/>
     </row>
-    <row r="615" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="615" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B615" s="1"/>
     </row>
-    <row r="616" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="616" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B616" s="1"/>
     </row>
-    <row r="617" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="617" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B617" s="1"/>
     </row>
-    <row r="618" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="618" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B618" s="1"/>
     </row>
-    <row r="619" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="619" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B619" s="1"/>
     </row>
-    <row r="620" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="620" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B620" s="1"/>
     </row>
-    <row r="621" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="621" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B621" s="1"/>
     </row>
-    <row r="622" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="622" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B622" s="1"/>
     </row>
-    <row r="623" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="623" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B623" s="1"/>
     </row>
-    <row r="624" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="624" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B624" s="1"/>
     </row>
-    <row r="625" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="625" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B625" s="1"/>
     </row>
-    <row r="626" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="626" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B626" s="1"/>
     </row>
-    <row r="627" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="627" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B627" s="1"/>
     </row>
-    <row r="628" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="628" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B628" s="1"/>
     </row>
-    <row r="629" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="629" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B629" s="1"/>
     </row>
-    <row r="630" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="630" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B630" s="1"/>
     </row>
-    <row r="631" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="631" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B631" s="1"/>
     </row>
-    <row r="632" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="632" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B632" s="1"/>
     </row>
-    <row r="633" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="633" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B633" s="1"/>
     </row>
-    <row r="634" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="634" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B634" s="1"/>
     </row>
-    <row r="635" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="635" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B635" s="1"/>
     </row>
-    <row r="636" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="636" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B636" s="1"/>
     </row>
-    <row r="637" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="637" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B637" s="1"/>
     </row>
-    <row r="638" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="638" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B638" s="1"/>
     </row>
-    <row r="639" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="639" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B639" s="1"/>
     </row>
-    <row r="640" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="640" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B640" s="1"/>
     </row>
-    <row r="641" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="641" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B641" s="1"/>
     </row>
-    <row r="642" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="642" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B642" s="1"/>
     </row>
-    <row r="643" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="643" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B643" s="1"/>
     </row>
-    <row r="644" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="644" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B644" s="1"/>
     </row>
-    <row r="645" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="645" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B645" s="1"/>
     </row>
-    <row r="646" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="646" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B646" s="1"/>
     </row>
-    <row r="647" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="647" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B647" s="1"/>
     </row>
-    <row r="648" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="648" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B648" s="1"/>
     </row>
-    <row r="649" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="649" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B649" s="1"/>
     </row>
-    <row r="650" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="650" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B650" s="1"/>
     </row>
-    <row r="651" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="651" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B651" s="1"/>
     </row>
-    <row r="652" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="652" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B652" s="1"/>
     </row>
-    <row r="653" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="653" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B653" s="1"/>
     </row>
-    <row r="654" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="654" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B654" s="1"/>
     </row>
-    <row r="655" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="655" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B655" s="1"/>
     </row>
-    <row r="656" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="656" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B656" s="1"/>
     </row>
-    <row r="657" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="657" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B657" s="1"/>
     </row>
-    <row r="658" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="658" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B658" s="1"/>
     </row>
-    <row r="659" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="659" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B659" s="1"/>
     </row>
-    <row r="660" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="660" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B660" s="1"/>
     </row>
-    <row r="661" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="661" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B661" s="1"/>
     </row>
-    <row r="662" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="662" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B662" s="1"/>
     </row>
-    <row r="663" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="663" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B663" s="1"/>
     </row>
-    <row r="664" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="664" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B664" s="1"/>
     </row>
-    <row r="665" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="665" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B665" s="1"/>
     </row>
-    <row r="666" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="666" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B666" s="1"/>
     </row>
-    <row r="667" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="667" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B667" s="1"/>
     </row>
-    <row r="668" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="668" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B668" s="1"/>
     </row>
-    <row r="669" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="669" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B669" s="1"/>
     </row>
-    <row r="670" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="670" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B670" s="1"/>
     </row>
-    <row r="671" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="671" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B671" s="1"/>
     </row>
-    <row r="672" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="672" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B672" s="1"/>
     </row>
-    <row r="673" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="673" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B673" s="1"/>
     </row>
-    <row r="674" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="674" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B674" s="1"/>
     </row>
-    <row r="675" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="675" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B675" s="1"/>
     </row>
-    <row r="676" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="676" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B676" s="1"/>
     </row>
-    <row r="677" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="677" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B677" s="1"/>
     </row>
-    <row r="678" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="678" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B678" s="1"/>
     </row>
-    <row r="679" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="679" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B679" s="1"/>
     </row>
-    <row r="680" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="680" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B680" s="1"/>
     </row>
-    <row r="681" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="681" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B681" s="1"/>
     </row>
-    <row r="682" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="682" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B682" s="1"/>
     </row>
-    <row r="683" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="683" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B683" s="1"/>
     </row>
-    <row r="684" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="684" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B684" s="1"/>
     </row>
-    <row r="685" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="685" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B685" s="1"/>
     </row>
-    <row r="686" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="686" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B686" s="1"/>
     </row>
-    <row r="687" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="687" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B687" s="1"/>
     </row>
-    <row r="688" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="688" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B688" s="1"/>
     </row>
-    <row r="689" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="689" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B689" s="1"/>
     </row>
-    <row r="690" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="690" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B690" s="1"/>
     </row>
-    <row r="691" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="691" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B691" s="1"/>
     </row>
-    <row r="692" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="692" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B692" s="1"/>
     </row>
-    <row r="693" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="693" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B693" s="1"/>
     </row>
-    <row r="694" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="694" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B694" s="1"/>
     </row>
-    <row r="695" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="695" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B695" s="1"/>
     </row>
-    <row r="696" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="696" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B696" s="1"/>
     </row>
-    <row r="697" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="697" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B697" s="1"/>
     </row>
-    <row r="698" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="698" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B698" s="1"/>
     </row>
-    <row r="699" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="699" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B699" s="1"/>
     </row>
-    <row r="700" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="700" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B700" s="1"/>
     </row>
-    <row r="701" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="701" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B701" s="1"/>
     </row>
-    <row r="702" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="702" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B702" s="1"/>
     </row>
-    <row r="703" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="703" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B703" s="1"/>
     </row>
-    <row r="704" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="704" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B704" s="1"/>
     </row>
-    <row r="705" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="705" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B705" s="1"/>
     </row>
-    <row r="706" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="706" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B706" s="1"/>
     </row>
-    <row r="707" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="707" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B707" s="1"/>
     </row>
-    <row r="708" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="708" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B708" s="1"/>
     </row>
-    <row r="709" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="709" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B709" s="1"/>
     </row>
-    <row r="710" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="710" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B710" s="1"/>
     </row>
-    <row r="711" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="711" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B711" s="1"/>
     </row>
-    <row r="712" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="712" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B712" s="1"/>
     </row>
-    <row r="713" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="713" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B713" s="1"/>
     </row>
-    <row r="714" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="714" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B714" s="1"/>
     </row>
-    <row r="715" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="715" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B715" s="1"/>
     </row>
-    <row r="716" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="716" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B716" s="1"/>
     </row>
-    <row r="717" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="717" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B717" s="1"/>
     </row>
-    <row r="718" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="718" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B718" s="1"/>
     </row>
-    <row r="719" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="719" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B719" s="1"/>
     </row>
-    <row r="720" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="720" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B720" s="1"/>
     </row>
-    <row r="721" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="721" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B721" s="1"/>
     </row>
-    <row r="722" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="722" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B722" s="1"/>
     </row>
-    <row r="723" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="723" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B723" s="1"/>
     </row>
-    <row r="724" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="724" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B724" s="1"/>
     </row>
-    <row r="725" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="725" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B725" s="1"/>
     </row>
-    <row r="726" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="726" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B726" s="1"/>
     </row>
-    <row r="727" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="727" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B727" s="1"/>
     </row>
-    <row r="728" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="728" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B728" s="1"/>
     </row>
-    <row r="729" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="729" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B729" s="1"/>
     </row>
-    <row r="730" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="730" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B730" s="1"/>
     </row>
-    <row r="731" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="731" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B731" s="1"/>
     </row>
-    <row r="732" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="732" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B732" s="1"/>
     </row>
-    <row r="733" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="733" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B733" s="1"/>
     </row>
-    <row r="734" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="734" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B734" s="1"/>
     </row>
-    <row r="735" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="735" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B735" s="1"/>
     </row>
-    <row r="736" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="736" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B736" s="1"/>
     </row>
-    <row r="737" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="737" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B737" s="1"/>
     </row>
-    <row r="738" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="738" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B738" s="1"/>
     </row>
-    <row r="739" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="739" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B739" s="1"/>
     </row>
-    <row r="740" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="740" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B740" s="1"/>
     </row>
-    <row r="741" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="741" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B741" s="1"/>
     </row>
-    <row r="742" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="742" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B742" s="1"/>
     </row>
-    <row r="743" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="743" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B743" s="1"/>
     </row>
-    <row r="744" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="744" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B744" s="1"/>
     </row>
-    <row r="745" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="745" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B745" s="1"/>
     </row>
-    <row r="746" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="746" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B746" s="1"/>
     </row>
-    <row r="747" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="747" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B747" s="1"/>
     </row>
-    <row r="748" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="748" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B748" s="1"/>
     </row>
-    <row r="749" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="749" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B749" s="1"/>
     </row>
-    <row r="750" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="750" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B750" s="1"/>
     </row>
-    <row r="751" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="751" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B751" s="1"/>
     </row>
-    <row r="752" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="752" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B752" s="1"/>
     </row>
-    <row r="753" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="753" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B753" s="1"/>
     </row>
-    <row r="754" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="754" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B754" s="1"/>
     </row>
-    <row r="755" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="755" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B755" s="1"/>
     </row>
-    <row r="756" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="756" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B756" s="1"/>
     </row>
-    <row r="757" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="757" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B757" s="1"/>
     </row>
-    <row r="758" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="758" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B758" s="1"/>
     </row>
-    <row r="759" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="759" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B759" s="1"/>
     </row>
-    <row r="760" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="760" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B760" s="1"/>
     </row>
-    <row r="761" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="761" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B761" s="1"/>
     </row>
-    <row r="762" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="762" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B762" s="1"/>
     </row>
-    <row r="763" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="763" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B763" s="1"/>
     </row>
-    <row r="764" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="764" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B764" s="1"/>
     </row>
-    <row r="765" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="765" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B765" s="1"/>
     </row>
-    <row r="766" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="766" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B766" s="1"/>
     </row>
-    <row r="767" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="767" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B767" s="1"/>
     </row>
-    <row r="768" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="768" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B768" s="1"/>
     </row>
-    <row r="769" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="769" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B769" s="1"/>
     </row>
-    <row r="770" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="770" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B770" s="1"/>
     </row>
-    <row r="771" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="771" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B771" s="1"/>
     </row>
-    <row r="772" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="772" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B772" s="1"/>
     </row>
-    <row r="773" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="773" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B773" s="1"/>
     </row>
-    <row r="774" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="774" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B774" s="1"/>
     </row>
-    <row r="775" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="775" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B775" s="1"/>
     </row>
-    <row r="776" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="776" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B776" s="1"/>
     </row>
-    <row r="777" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="777" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B777" s="1"/>
     </row>
-    <row r="778" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="778" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B778" s="1"/>
     </row>
-    <row r="779" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="779" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B779" s="1"/>
     </row>
-    <row r="780" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="780" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B780" s="1"/>
     </row>
-    <row r="781" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="781" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B781" s="1"/>
     </row>
-    <row r="782" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="782" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B782" s="1"/>
     </row>
-    <row r="783" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="783" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B783" s="1"/>
     </row>
-    <row r="784" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="784" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B784" s="1"/>
     </row>
-    <row r="785" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="785" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B785" s="1"/>
     </row>
-    <row r="786" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="786" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B786" s="1"/>
     </row>
-    <row r="787" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="787" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B787" s="1"/>
     </row>
-    <row r="788" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="788" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B788" s="1"/>
     </row>
-    <row r="789" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="789" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B789" s="1"/>
     </row>
-    <row r="790" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="790" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B790" s="1"/>
     </row>
-    <row r="791" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="791" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B791" s="1"/>
     </row>
-    <row r="792" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="792" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B792" s="1"/>
     </row>
-    <row r="793" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="793" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B793" s="1"/>
     </row>
-    <row r="794" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="794" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B794" s="1"/>
     </row>
-    <row r="795" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="795" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B795" s="1"/>
     </row>
-    <row r="796" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="796" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B796" s="1"/>
     </row>
-    <row r="797" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="797" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B797" s="1"/>
     </row>
-    <row r="798" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="798" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B798" s="1"/>
     </row>
-    <row r="799" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="799" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B799" s="1"/>
     </row>
-    <row r="800" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="800" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B800" s="1"/>
     </row>
-    <row r="801" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="801" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B801" s="1"/>
     </row>
-    <row r="802" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="802" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B802" s="1"/>
     </row>
-    <row r="803" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="803" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B803" s="1"/>
     </row>
-    <row r="804" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="804" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B804" s="1"/>
     </row>
-    <row r="805" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="805" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B805" s="1"/>
     </row>
-    <row r="806" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="806" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B806" s="1"/>
     </row>
-    <row r="807" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="807" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B807" s="1"/>
     </row>
-    <row r="808" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="808" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B808" s="1"/>
     </row>
-    <row r="809" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="809" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B809" s="1"/>
     </row>
-    <row r="810" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="810" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B810" s="1"/>
     </row>
-    <row r="811" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="811" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B811" s="1"/>
     </row>
-    <row r="812" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="812" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B812" s="1"/>
     </row>
-    <row r="813" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="813" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B813" s="1"/>
     </row>
-    <row r="814" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="814" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B814" s="1"/>
     </row>
-    <row r="815" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="815" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B815" s="1"/>
     </row>
-    <row r="816" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="816" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B816" s="1"/>
     </row>
-    <row r="817" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="817" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B817" s="1"/>
     </row>
-    <row r="818" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="818" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B818" s="1"/>
     </row>
-    <row r="819" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="819" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B819" s="1"/>
     </row>
-    <row r="820" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="820" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B820" s="1"/>
     </row>
-    <row r="821" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="821" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B821" s="1"/>
     </row>
-    <row r="822" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="822" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B822" s="1"/>
     </row>
-    <row r="823" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="823" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B823" s="1"/>
     </row>
-    <row r="824" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="824" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B824" s="1"/>
     </row>
-    <row r="825" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="825" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B825" s="1"/>
     </row>
-    <row r="826" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="826" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B826" s="1"/>
     </row>
-    <row r="827" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="827" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B827" s="1"/>
     </row>
-    <row r="828" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="828" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B828" s="1"/>
     </row>
-    <row r="829" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="829" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B829" s="1"/>
     </row>
-    <row r="830" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="830" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B830" s="1"/>
     </row>
-    <row r="831" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="831" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B831" s="1"/>
     </row>
-    <row r="832" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="832" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B832" s="1"/>
     </row>
-    <row r="833" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="833" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B833" s="1"/>
     </row>
-    <row r="834" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="834" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B834" s="1"/>
     </row>
-    <row r="835" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="835" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B835" s="1"/>
     </row>
-    <row r="836" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="836" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B836" s="1"/>
     </row>
-    <row r="837" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="837" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B837" s="1"/>
     </row>
-    <row r="838" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="838" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B838" s="1"/>
     </row>
-    <row r="839" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="839" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B839" s="1"/>
     </row>
-    <row r="840" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="840" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B840" s="1"/>
     </row>
-    <row r="841" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="841" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B841" s="1"/>
     </row>
-    <row r="842" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="842" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B842" s="1"/>
     </row>
-    <row r="843" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="843" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B843" s="1"/>
     </row>
-    <row r="844" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="844" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B844" s="1"/>
     </row>
-    <row r="845" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="845" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B845" s="1"/>
     </row>
-    <row r="846" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="846" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B846" s="1"/>
     </row>
-    <row r="847" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="847" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B847" s="1"/>
     </row>
-    <row r="848" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="848" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B848" s="1"/>
     </row>
-    <row r="849" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="849" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B849" s="1"/>
     </row>
-    <row r="850" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="850" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B850" s="1"/>
     </row>
-    <row r="851" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="851" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B851" s="1"/>
     </row>
-    <row r="852" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="852" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B852" s="1"/>
     </row>
-    <row r="853" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="853" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B853" s="1"/>
     </row>
-    <row r="854" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="854" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B854" s="1"/>
     </row>
-    <row r="855" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="855" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B855" s="1"/>
     </row>
-    <row r="856" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="856" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B856" s="1"/>
     </row>
-    <row r="857" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="857" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B857" s="1"/>
     </row>
-    <row r="858" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="858" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B858" s="1"/>
     </row>
-    <row r="859" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="859" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B859" s="1"/>
     </row>
-    <row r="860" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="860" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B860" s="1"/>
     </row>
-    <row r="861" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="861" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B861" s="1"/>
     </row>
-    <row r="862" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="862" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B862" s="1"/>
     </row>
-    <row r="863" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="863" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B863" s="1"/>
     </row>
-    <row r="864" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="864" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B864" s="1"/>
     </row>
-    <row r="865" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="865" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B865" s="1"/>
     </row>
-    <row r="866" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="866" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B866" s="1"/>
     </row>
-    <row r="867" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="867" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B867" s="1"/>
     </row>
-    <row r="868" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="868" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B868" s="1"/>
     </row>
-    <row r="869" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="869" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B869" s="1"/>
     </row>
-    <row r="870" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="870" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B870" s="1"/>
     </row>
-    <row r="871" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="871" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B871" s="1"/>
     </row>
-    <row r="872" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="872" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B872" s="1"/>
     </row>
-    <row r="873" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="873" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B873" s="1"/>
     </row>
-    <row r="874" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="874" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B874" s="1"/>
     </row>
-    <row r="875" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="875" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B875" s="1"/>
     </row>
-    <row r="876" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="876" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B876" s="1"/>
     </row>
-    <row r="877" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="877" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B877" s="1"/>
     </row>
-    <row r="878" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="878" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B878" s="1"/>
     </row>
-    <row r="879" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="879" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B879" s="1"/>
     </row>
-    <row r="880" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="880" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B880" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F882">
+  <sortState ref="A1:F882">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
toast en la aplicación, consulta de personal por IE para el administardor, páginación en toda la aplicación, inclución de select2 en el formulario de buscar personal por IE y en el formulario de crear usuario
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61776037-745C-41EE-96F8-3AD078A3271B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEF345-8CAA-457F-BEB3-6F9E7133149E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
   <si>
     <t>a</t>
   </si>
@@ -865,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F880"/>
+  <dimension ref="A1:F883"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,10 +879,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>45728.33011574074</v>
+        <v>45747.33011574074</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>45728.54446759259</v>
+        <v>45747.337060185186</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>45729.330474537041</v>
+        <v>45747.545393518521</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>45729.544317129628</v>
+        <v>45747.550949074073</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>45729.591249999998</v>
+        <v>45747.591921296298</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -979,10 +979,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>45729.733657407407</v>
+        <v>45747.59747685185</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -999,10 +999,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>45730.326597222222</v>
+        <v>45747.746782407405</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1019,10 +1019,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>45730.563738425924</v>
+        <v>45747.748171296298</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1038,701 +1038,123 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45731.32671296296</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45731.545347222222</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45731.585497685184</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45731.7809375</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45732.327685185184</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45732.546666666669</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1">
-        <v>45732.587546296294</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45732.745439814818</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
-        <v>45733.328090277777</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
-        <v>45733.593657407408</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
-        <v>45733.757013888891</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45734.328923611109</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1">
-        <v>45728.33011574074</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1">
-        <v>45728.54446759259</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" s="1">
-        <v>45729.330474537041</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1">
-        <v>45729.544317129628</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" s="1">
-        <v>45729.591249999998</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1">
-        <v>45729.733657407407</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" s="1">
-        <v>45730.326597222222</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="1">
-        <v>45730.563738425924</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" s="1">
-        <v>45731.32671296296</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" s="1">
-        <v>45731.545347222222</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1">
-        <v>45731.585497685184</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1">
-        <v>45731.7809375</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1">
-        <v>45732.327685185184</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45732.546666666669</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" s="1">
-        <v>45732.587546296294</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36" s="1">
-        <v>45732.745439814818</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" s="1">
-        <v>45733.328090277777</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2</v>
-      </c>
-      <c r="B38" s="1">
-        <v>45733.593657407408</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45733.757013888891</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2</v>
-      </c>
-      <c r="B40" s="1">
-        <v>45734.328923611109</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" s="1">
-        <v>45734.578923611109</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42" s="1">
-        <v>45734.74559027778</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -4231,8 +3653,17 @@
     <row r="880" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B880" s="1"/>
     </row>
+    <row r="881" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B881" s="1"/>
+    </row>
+    <row r="882" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B882" s="1"/>
+    </row>
+    <row r="883" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B883" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:F882">
+  <sortState ref="A1:F885">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
botón de eliminar registro de asistencia visible solo durante 24 horas después de su registro
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEF345-8CAA-457F-BEB3-6F9E7133149E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F56FF-438E-4C95-B429-5C0DC515993D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -868,7 +868,7 @@
   <dimension ref="A1:F883"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +882,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>45747.33011574074</v>
+        <v>45748.33011574074</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>45747.337060185186</v>
+        <v>45748.337060185186</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>45747.545393518521</v>
+        <v>45748.545393518521</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -942,7 +942,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>45747.550949074073</v>
+        <v>45748.550949074073</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>45747.591921296298</v>
+        <v>45748.591921296298</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>45747.59747685185</v>
+        <v>45748.59747685185</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>45747.746782407405</v>
+        <v>45748.746782407405</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1022,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>45747.748171296298</v>
+        <v>45748.748171296298</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
manejo de horarios por turnos de personal en las vistas de los reportes, mejora en el manejo de rol y turnoIE  en las vistas
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F56FF-438E-4C95-B429-5C0DC515993D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E256B1AF-19F6-4CEB-91FF-0B8D7A5663C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVG231060035_attlog" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
   <dimension ref="A1:F883"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,10 +879,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>45748.33011574074</v>
+        <v>45753.788449074076</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45748.337060185186</v>
+        <v>45753.962060185186</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>45748.545393518521</v>
+        <v>45753.75372685185</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>45748.550949074073</v>
+        <v>45753.957199074073</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>45748.591921296298</v>
+        <v>45753.959976851853</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>45748.59747685185</v>
+        <v>45752.764143518521</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>45748.746782407405</v>
+        <v>45753.957199074073</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1022,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>45748.748171296298</v>
+        <v>45753.949560185189</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
cambio en la función para covertir las fechas a excel
</commit_message>
<xml_diff>
--- a/src/archives/asistencia.xlsx
+++ b/src/archives/asistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\yoxer\PROYECTOS DESARROLLADOS\UGEL HBBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E256B1AF-19F6-4CEB-91FF-0B8D7A5663C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2F389-8BA9-4F11-A0D1-5A2D1E49F095}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
-  <si>
-    <t>a</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -165,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +341,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -506,10 +508,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -865,16 +868,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F883"/>
+  <dimension ref="A1:F2203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>45753.788449074076</v>
+        <v>45728.327326388891</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
+      <c r="C1">
+        <v>1</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -902,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45753.962060185186</v>
+        <v>45728.544189814813</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -918,34 +920,34 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="2">
+        <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>45753.75372685185</v>
+      <c r="B3" s="3">
+        <v>45728.581296296295</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="E3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="B4" s="1">
+        <v>45729.004791666666</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45753.957199074073</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -958,34 +960,34 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
+      <c r="A5" s="2">
+        <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>45753.959976851853</v>
+      <c r="B5" s="3">
+        <v>45729.328958333332</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="E5">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="B6" s="1">
+        <v>45729.545104166667</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45752.764143518521</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -999,13 +1001,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>45753.957199074073</v>
+        <v>45729.593935185185</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1019,13 +1021,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>45753.949560185189</v>
+        <v>45729.87159722222</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1235,8 +1237,8 @@
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
+    <row r="75" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
@@ -1673,8 +1675,8 @@
     <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="1"/>
+    <row r="221" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B221" s="3"/>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" s="1"/>
@@ -2039,11 +2041,11 @@
     <row r="342" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B342" s="1"/>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B343" s="1"/>
-    </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B344" s="1"/>
+    <row r="343" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B343" s="3"/>
+    </row>
+    <row r="344" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B344" s="3"/>
     </row>
     <row r="345" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B345" s="1"/>
@@ -2480,8 +2482,8 @@
     <row r="489" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B489" s="1"/>
     </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B490" s="1"/>
+    <row r="490" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B490" s="3"/>
     </row>
     <row r="491" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B491" s="1"/>
@@ -2906,8 +2908,8 @@
     <row r="631" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B631" s="1"/>
     </row>
-    <row r="632" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B632" s="1"/>
+    <row r="632" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B632" s="3"/>
     </row>
     <row r="633" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B633" s="1"/>
@@ -3416,8 +3418,8 @@
     <row r="801" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B801" s="1"/>
     </row>
-    <row r="802" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B802" s="1"/>
+    <row r="802" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B802" s="3"/>
     </row>
     <row r="803" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B803" s="1"/>
@@ -3662,10 +3664,3967 @@
     <row r="883" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B883" s="1"/>
     </row>
+    <row r="884" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B884" s="1"/>
+    </row>
+    <row r="885" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B885" s="1"/>
+    </row>
+    <row r="886" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B886" s="1"/>
+    </row>
+    <row r="887" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B887" s="1"/>
+    </row>
+    <row r="888" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B888" s="1"/>
+    </row>
+    <row r="889" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B889" s="1"/>
+    </row>
+    <row r="890" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B890" s="1"/>
+    </row>
+    <row r="891" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B891" s="1"/>
+    </row>
+    <row r="892" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B892" s="1"/>
+    </row>
+    <row r="893" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B893" s="1"/>
+    </row>
+    <row r="894" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B894" s="1"/>
+    </row>
+    <row r="895" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B895" s="1"/>
+    </row>
+    <row r="896" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B896" s="1"/>
+    </row>
+    <row r="897" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B897" s="1"/>
+    </row>
+    <row r="898" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B898" s="1"/>
+    </row>
+    <row r="899" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B899" s="1"/>
+    </row>
+    <row r="900" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B900" s="1"/>
+    </row>
+    <row r="901" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B901" s="1"/>
+    </row>
+    <row r="902" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B902" s="1"/>
+    </row>
+    <row r="903" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B903" s="1"/>
+    </row>
+    <row r="904" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B904" s="1"/>
+    </row>
+    <row r="905" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B905" s="1"/>
+    </row>
+    <row r="906" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B906" s="1"/>
+    </row>
+    <row r="907" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B907" s="1"/>
+    </row>
+    <row r="908" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B908" s="1"/>
+    </row>
+    <row r="909" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B909" s="1"/>
+    </row>
+    <row r="910" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B910" s="1"/>
+    </row>
+    <row r="911" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B911" s="1"/>
+    </row>
+    <row r="912" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B912" s="1"/>
+    </row>
+    <row r="913" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B913" s="1"/>
+    </row>
+    <row r="914" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B914" s="1"/>
+    </row>
+    <row r="915" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B915" s="1"/>
+    </row>
+    <row r="916" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B916" s="1"/>
+    </row>
+    <row r="917" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B917" s="1"/>
+    </row>
+    <row r="918" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B918" s="1"/>
+    </row>
+    <row r="919" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B919" s="1"/>
+    </row>
+    <row r="920" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B920" s="1"/>
+    </row>
+    <row r="921" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B921" s="1"/>
+    </row>
+    <row r="922" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B922" s="1"/>
+    </row>
+    <row r="923" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B923" s="1"/>
+    </row>
+    <row r="924" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B924" s="1"/>
+    </row>
+    <row r="925" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B925" s="1"/>
+    </row>
+    <row r="926" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B926" s="1"/>
+    </row>
+    <row r="927" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B927" s="1"/>
+    </row>
+    <row r="928" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B928" s="1"/>
+    </row>
+    <row r="929" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B929" s="1"/>
+    </row>
+    <row r="930" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B930" s="1"/>
+    </row>
+    <row r="931" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B931" s="1"/>
+    </row>
+    <row r="932" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B932" s="1"/>
+    </row>
+    <row r="933" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B933" s="1"/>
+    </row>
+    <row r="934" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B934" s="1"/>
+    </row>
+    <row r="935" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B935" s="1"/>
+    </row>
+    <row r="936" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B936" s="1"/>
+    </row>
+    <row r="937" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B937" s="1"/>
+    </row>
+    <row r="938" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B938" s="1"/>
+    </row>
+    <row r="939" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B939" s="1"/>
+    </row>
+    <row r="940" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B940" s="1"/>
+    </row>
+    <row r="941" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B941" s="1"/>
+    </row>
+    <row r="942" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B942" s="1"/>
+    </row>
+    <row r="943" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B943" s="1"/>
+    </row>
+    <row r="944" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B944" s="1"/>
+    </row>
+    <row r="945" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B945" s="1"/>
+    </row>
+    <row r="946" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B946" s="1"/>
+    </row>
+    <row r="947" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B947" s="1"/>
+    </row>
+    <row r="948" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B948" s="1"/>
+    </row>
+    <row r="949" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B949" s="1"/>
+    </row>
+    <row r="950" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B950" s="1"/>
+    </row>
+    <row r="951" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B951" s="1"/>
+    </row>
+    <row r="952" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B952" s="1"/>
+    </row>
+    <row r="953" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B953" s="1"/>
+    </row>
+    <row r="954" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B954" s="1"/>
+    </row>
+    <row r="955" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B955" s="1"/>
+    </row>
+    <row r="956" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B956" s="1"/>
+    </row>
+    <row r="957" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B957" s="1"/>
+    </row>
+    <row r="958" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B958" s="1"/>
+    </row>
+    <row r="959" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B959" s="1"/>
+    </row>
+    <row r="960" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B960" s="1"/>
+    </row>
+    <row r="961" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B961" s="1"/>
+    </row>
+    <row r="962" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B962" s="1"/>
+    </row>
+    <row r="963" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B963" s="1"/>
+    </row>
+    <row r="964" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B964" s="1"/>
+    </row>
+    <row r="965" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B965" s="1"/>
+    </row>
+    <row r="966" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B966" s="1"/>
+    </row>
+    <row r="967" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B967" s="1"/>
+    </row>
+    <row r="968" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B968" s="1"/>
+    </row>
+    <row r="969" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B969" s="1"/>
+    </row>
+    <row r="970" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B970" s="3"/>
+    </row>
+    <row r="971" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B971" s="1"/>
+    </row>
+    <row r="972" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B972" s="1"/>
+    </row>
+    <row r="973" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B973" s="1"/>
+    </row>
+    <row r="974" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B974" s="1"/>
+    </row>
+    <row r="975" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B975" s="1"/>
+    </row>
+    <row r="976" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B976" s="1"/>
+    </row>
+    <row r="977" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B977" s="1"/>
+    </row>
+    <row r="978" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B978" s="1"/>
+    </row>
+    <row r="979" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B979" s="1"/>
+    </row>
+    <row r="980" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B980" s="1"/>
+    </row>
+    <row r="981" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B981" s="1"/>
+    </row>
+    <row r="982" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B982" s="1"/>
+    </row>
+    <row r="983" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B983" s="1"/>
+    </row>
+    <row r="984" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B984" s="1"/>
+    </row>
+    <row r="985" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B985" s="1"/>
+    </row>
+    <row r="986" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B986" s="1"/>
+    </row>
+    <row r="987" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B987" s="1"/>
+    </row>
+    <row r="988" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B988" s="1"/>
+    </row>
+    <row r="989" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B989" s="1"/>
+    </row>
+    <row r="990" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B990" s="1"/>
+    </row>
+    <row r="991" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B991" s="1"/>
+    </row>
+    <row r="992" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B992" s="1"/>
+    </row>
+    <row r="993" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B993" s="1"/>
+    </row>
+    <row r="994" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B994" s="1"/>
+    </row>
+    <row r="995" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B995" s="1"/>
+    </row>
+    <row r="996" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B996" s="1"/>
+    </row>
+    <row r="997" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B997" s="1"/>
+    </row>
+    <row r="998" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B998" s="1"/>
+    </row>
+    <row r="999" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B999" s="1"/>
+    </row>
+    <row r="1000" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1000" s="1"/>
+    </row>
+    <row r="1001" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1001" s="1"/>
+    </row>
+    <row r="1002" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1002" s="1"/>
+    </row>
+    <row r="1003" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1003" s="1"/>
+    </row>
+    <row r="1004" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1004" s="1"/>
+    </row>
+    <row r="1005" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1005" s="1"/>
+    </row>
+    <row r="1006" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1006" s="1"/>
+    </row>
+    <row r="1007" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1007" s="1"/>
+    </row>
+    <row r="1008" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1008" s="1"/>
+    </row>
+    <row r="1009" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1009" s="1"/>
+    </row>
+    <row r="1010" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1010" s="1"/>
+    </row>
+    <row r="1011" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1011" s="1"/>
+    </row>
+    <row r="1012" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1012" s="1"/>
+    </row>
+    <row r="1013" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1013" s="1"/>
+    </row>
+    <row r="1014" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1014" s="1"/>
+    </row>
+    <row r="1015" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1015" s="1"/>
+    </row>
+    <row r="1016" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1016" s="1"/>
+    </row>
+    <row r="1017" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1017" s="1"/>
+    </row>
+    <row r="1018" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1018" s="1"/>
+    </row>
+    <row r="1019" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1019" s="1"/>
+    </row>
+    <row r="1020" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1020" s="1"/>
+    </row>
+    <row r="1021" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1021" s="1"/>
+    </row>
+    <row r="1022" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1022" s="1"/>
+    </row>
+    <row r="1023" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1023" s="1"/>
+    </row>
+    <row r="1024" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1024" s="1"/>
+    </row>
+    <row r="1025" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1025" s="1"/>
+    </row>
+    <row r="1026" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1026" s="1"/>
+    </row>
+    <row r="1027" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1027" s="1"/>
+    </row>
+    <row r="1028" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1028" s="1"/>
+    </row>
+    <row r="1029" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1029" s="1"/>
+    </row>
+    <row r="1030" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1030" s="1"/>
+    </row>
+    <row r="1031" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1031" s="1"/>
+    </row>
+    <row r="1032" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1032" s="1"/>
+    </row>
+    <row r="1033" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1033" s="1"/>
+    </row>
+    <row r="1034" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1034" s="1"/>
+    </row>
+    <row r="1035" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1035" s="1"/>
+    </row>
+    <row r="1036" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1036" s="1"/>
+    </row>
+    <row r="1037" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1037" s="1"/>
+    </row>
+    <row r="1038" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1038" s="1"/>
+    </row>
+    <row r="1039" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1039" s="1"/>
+    </row>
+    <row r="1040" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1040" s="1"/>
+    </row>
+    <row r="1041" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1041" s="1"/>
+    </row>
+    <row r="1042" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1042" s="1"/>
+    </row>
+    <row r="1043" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1043" s="1"/>
+    </row>
+    <row r="1044" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1044" s="1"/>
+    </row>
+    <row r="1045" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1045" s="1"/>
+    </row>
+    <row r="1046" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1046" s="1"/>
+    </row>
+    <row r="1047" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1047" s="1"/>
+    </row>
+    <row r="1048" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1048" s="1"/>
+    </row>
+    <row r="1049" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1049" s="1"/>
+    </row>
+    <row r="1050" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1050" s="1"/>
+    </row>
+    <row r="1051" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1051" s="1"/>
+    </row>
+    <row r="1052" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1052" s="1"/>
+    </row>
+    <row r="1053" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1053" s="1"/>
+    </row>
+    <row r="1054" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1054" s="1"/>
+    </row>
+    <row r="1055" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1055" s="1"/>
+    </row>
+    <row r="1056" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1056" s="1"/>
+    </row>
+    <row r="1057" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1057" s="1"/>
+    </row>
+    <row r="1058" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1058" s="1"/>
+    </row>
+    <row r="1059" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1059" s="1"/>
+    </row>
+    <row r="1060" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1060" s="1"/>
+    </row>
+    <row r="1061" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1061" s="1"/>
+    </row>
+    <row r="1062" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1062" s="1"/>
+    </row>
+    <row r="1063" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1063" s="1"/>
+    </row>
+    <row r="1064" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1064" s="1"/>
+    </row>
+    <row r="1065" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1065" s="1"/>
+    </row>
+    <row r="1066" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1066" s="1"/>
+    </row>
+    <row r="1067" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1067" s="1"/>
+    </row>
+    <row r="1068" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1068" s="1"/>
+    </row>
+    <row r="1069" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1069" s="1"/>
+    </row>
+    <row r="1070" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1070" s="1"/>
+    </row>
+    <row r="1071" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1071" s="1"/>
+    </row>
+    <row r="1072" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1072" s="1"/>
+    </row>
+    <row r="1073" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1073" s="1"/>
+    </row>
+    <row r="1074" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1074" s="1"/>
+    </row>
+    <row r="1075" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1075" s="1"/>
+    </row>
+    <row r="1076" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1076" s="1"/>
+    </row>
+    <row r="1077" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1077" s="1"/>
+    </row>
+    <row r="1078" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1078" s="1"/>
+    </row>
+    <row r="1079" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1079" s="1"/>
+    </row>
+    <row r="1080" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1080" s="1"/>
+    </row>
+    <row r="1081" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1081" s="1"/>
+    </row>
+    <row r="1082" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1082" s="1"/>
+    </row>
+    <row r="1083" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1083" s="1"/>
+    </row>
+    <row r="1084" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1084" s="1"/>
+    </row>
+    <row r="1085" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1085" s="1"/>
+    </row>
+    <row r="1086" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1086" s="1"/>
+    </row>
+    <row r="1087" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1087" s="1"/>
+    </row>
+    <row r="1088" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1088" s="1"/>
+    </row>
+    <row r="1089" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1089" s="1"/>
+    </row>
+    <row r="1090" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1090" s="1"/>
+    </row>
+    <row r="1091" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1091" s="1"/>
+    </row>
+    <row r="1092" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1092" s="1"/>
+    </row>
+    <row r="1093" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1093" s="1"/>
+    </row>
+    <row r="1094" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1094" s="1"/>
+    </row>
+    <row r="1095" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1095" s="1"/>
+    </row>
+    <row r="1096" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1096" s="1"/>
+    </row>
+    <row r="1097" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1097" s="1"/>
+    </row>
+    <row r="1098" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1098" s="1"/>
+    </row>
+    <row r="1099" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1099" s="1"/>
+    </row>
+    <row r="1100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1100" s="1"/>
+    </row>
+    <row r="1101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1101" s="1"/>
+    </row>
+    <row r="1102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1102" s="1"/>
+    </row>
+    <row r="1103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1103" s="1"/>
+    </row>
+    <row r="1104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1104" s="1"/>
+    </row>
+    <row r="1105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1105" s="1"/>
+    </row>
+    <row r="1106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1106" s="1"/>
+    </row>
+    <row r="1107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1107" s="1"/>
+    </row>
+    <row r="1108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1108" s="1"/>
+    </row>
+    <row r="1109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1109" s="1"/>
+    </row>
+    <row r="1110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1110" s="1"/>
+    </row>
+    <row r="1111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1111" s="1"/>
+    </row>
+    <row r="1112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1112" s="1"/>
+    </row>
+    <row r="1113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1113" s="1"/>
+    </row>
+    <row r="1114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1114" s="1"/>
+    </row>
+    <row r="1115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1115" s="1"/>
+    </row>
+    <row r="1116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1116" s="1"/>
+    </row>
+    <row r="1117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1117" s="1"/>
+    </row>
+    <row r="1118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1118" s="1"/>
+    </row>
+    <row r="1119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1119" s="1"/>
+    </row>
+    <row r="1120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1120" s="1"/>
+    </row>
+    <row r="1121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1121" s="1"/>
+    </row>
+    <row r="1122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1122" s="1"/>
+    </row>
+    <row r="1123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1123" s="1"/>
+    </row>
+    <row r="1124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1124" s="1"/>
+    </row>
+    <row r="1125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1125" s="1"/>
+    </row>
+    <row r="1126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1126" s="1"/>
+    </row>
+    <row r="1127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1127" s="1"/>
+    </row>
+    <row r="1128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1128" s="1"/>
+    </row>
+    <row r="1129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1129" s="1"/>
+    </row>
+    <row r="1130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1130" s="1"/>
+    </row>
+    <row r="1131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1131" s="1"/>
+    </row>
+    <row r="1132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1132" s="1"/>
+    </row>
+    <row r="1133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1133" s="1"/>
+    </row>
+    <row r="1134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1134" s="1"/>
+    </row>
+    <row r="1135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1135" s="1"/>
+    </row>
+    <row r="1136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1136" s="1"/>
+    </row>
+    <row r="1137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1137" s="1"/>
+    </row>
+    <row r="1138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1138" s="1"/>
+    </row>
+    <row r="1139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1139" s="1"/>
+    </row>
+    <row r="1140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1140" s="1"/>
+    </row>
+    <row r="1141" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1141" s="3"/>
+    </row>
+    <row r="1142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1142" s="1"/>
+    </row>
+    <row r="1143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1143" s="1"/>
+    </row>
+    <row r="1144" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1144" s="3"/>
+    </row>
+    <row r="1145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1145" s="1"/>
+    </row>
+    <row r="1146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1146" s="1"/>
+    </row>
+    <row r="1147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1147" s="1"/>
+    </row>
+    <row r="1148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1148" s="1"/>
+    </row>
+    <row r="1149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1149" s="1"/>
+    </row>
+    <row r="1150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1150" s="1"/>
+    </row>
+    <row r="1151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1151" s="1"/>
+    </row>
+    <row r="1152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1152" s="1"/>
+    </row>
+    <row r="1153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1153" s="1"/>
+    </row>
+    <row r="1154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1154" s="1"/>
+    </row>
+    <row r="1155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1155" s="1"/>
+    </row>
+    <row r="1156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1156" s="1"/>
+    </row>
+    <row r="1157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1157" s="1"/>
+    </row>
+    <row r="1158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1158" s="1"/>
+    </row>
+    <row r="1159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1159" s="1"/>
+    </row>
+    <row r="1160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1160" s="1"/>
+    </row>
+    <row r="1161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1161" s="1"/>
+    </row>
+    <row r="1162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1162" s="1"/>
+    </row>
+    <row r="1163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1163" s="1"/>
+    </row>
+    <row r="1164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1164" s="1"/>
+    </row>
+    <row r="1165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1165" s="1"/>
+    </row>
+    <row r="1166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1166" s="1"/>
+    </row>
+    <row r="1167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1167" s="1"/>
+    </row>
+    <row r="1168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1168" s="1"/>
+    </row>
+    <row r="1169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1169" s="1"/>
+    </row>
+    <row r="1170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1170" s="1"/>
+    </row>
+    <row r="1171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1171" s="1"/>
+    </row>
+    <row r="1172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1172" s="1"/>
+    </row>
+    <row r="1173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1173" s="1"/>
+    </row>
+    <row r="1174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1174" s="1"/>
+    </row>
+    <row r="1175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1175" s="1"/>
+    </row>
+    <row r="1176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1176" s="1"/>
+    </row>
+    <row r="1177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1177" s="1"/>
+    </row>
+    <row r="1178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1178" s="1"/>
+    </row>
+    <row r="1179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1179" s="1"/>
+    </row>
+    <row r="1180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1180" s="1"/>
+    </row>
+    <row r="1181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1181" s="1"/>
+    </row>
+    <row r="1182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1182" s="1"/>
+    </row>
+    <row r="1183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1183" s="1"/>
+    </row>
+    <row r="1184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1184" s="1"/>
+    </row>
+    <row r="1185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1185" s="1"/>
+    </row>
+    <row r="1186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1186" s="1"/>
+    </row>
+    <row r="1187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1187" s="1"/>
+    </row>
+    <row r="1188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1188" s="1"/>
+    </row>
+    <row r="1189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1189" s="1"/>
+    </row>
+    <row r="1190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1190" s="1"/>
+    </row>
+    <row r="1191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1191" s="1"/>
+    </row>
+    <row r="1192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1192" s="1"/>
+    </row>
+    <row r="1193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1193" s="1"/>
+    </row>
+    <row r="1194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1194" s="1"/>
+    </row>
+    <row r="1195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1195" s="1"/>
+    </row>
+    <row r="1196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1196" s="1"/>
+    </row>
+    <row r="1197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1197" s="1"/>
+    </row>
+    <row r="1198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1198" s="1"/>
+    </row>
+    <row r="1199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1199" s="1"/>
+    </row>
+    <row r="1200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1200" s="1"/>
+    </row>
+    <row r="1201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1201" s="1"/>
+    </row>
+    <row r="1202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1202" s="1"/>
+    </row>
+    <row r="1203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1203" s="1"/>
+    </row>
+    <row r="1204" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1204" s="1"/>
+    </row>
+    <row r="1205" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1205" s="1"/>
+    </row>
+    <row r="1206" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1206" s="1"/>
+    </row>
+    <row r="1207" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1207" s="1"/>
+    </row>
+    <row r="1208" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1208" s="1"/>
+    </row>
+    <row r="1209" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1209" s="1"/>
+    </row>
+    <row r="1210" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1210" s="1"/>
+    </row>
+    <row r="1211" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1211" s="1"/>
+    </row>
+    <row r="1212" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1212" s="1"/>
+    </row>
+    <row r="1213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1213" s="1"/>
+    </row>
+    <row r="1214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1214" s="1"/>
+    </row>
+    <row r="1215" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1215" s="1"/>
+    </row>
+    <row r="1216" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1216" s="1"/>
+    </row>
+    <row r="1217" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1217" s="1"/>
+    </row>
+    <row r="1218" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1218" s="1"/>
+    </row>
+    <row r="1219" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1219" s="1"/>
+    </row>
+    <row r="1220" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1220" s="1"/>
+    </row>
+    <row r="1221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1221" s="1"/>
+    </row>
+    <row r="1222" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1222" s="1"/>
+    </row>
+    <row r="1223" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1223" s="1"/>
+    </row>
+    <row r="1224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1224" s="1"/>
+    </row>
+    <row r="1225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1225" s="1"/>
+    </row>
+    <row r="1226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1226" s="1"/>
+    </row>
+    <row r="1227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1227" s="1"/>
+    </row>
+    <row r="1228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1228" s="1"/>
+    </row>
+    <row r="1229" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1229" s="1"/>
+    </row>
+    <row r="1230" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1230" s="1"/>
+    </row>
+    <row r="1231" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1231" s="1"/>
+    </row>
+    <row r="1232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1232" s="1"/>
+    </row>
+    <row r="1233" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1233" s="1"/>
+    </row>
+    <row r="1234" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1234" s="1"/>
+    </row>
+    <row r="1235" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1235" s="1"/>
+    </row>
+    <row r="1236" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1236" s="1"/>
+    </row>
+    <row r="1237" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1237" s="1"/>
+    </row>
+    <row r="1238" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1238" s="1"/>
+    </row>
+    <row r="1239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1239" s="1"/>
+    </row>
+    <row r="1240" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1240" s="1"/>
+    </row>
+    <row r="1241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1241" s="1"/>
+    </row>
+    <row r="1242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1242" s="1"/>
+    </row>
+    <row r="1243" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1243" s="3"/>
+    </row>
+    <row r="1244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1244" s="1"/>
+    </row>
+    <row r="1245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1245" s="1"/>
+    </row>
+    <row r="1246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1246" s="1"/>
+    </row>
+    <row r="1247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1247" s="1"/>
+    </row>
+    <row r="1248" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1248" s="1"/>
+    </row>
+    <row r="1249" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1249" s="1"/>
+    </row>
+    <row r="1250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1250" s="1"/>
+    </row>
+    <row r="1251" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1251" s="1"/>
+    </row>
+    <row r="1252" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1252" s="1"/>
+    </row>
+    <row r="1253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1253" s="1"/>
+    </row>
+    <row r="1254" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1254" s="1"/>
+    </row>
+    <row r="1255" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1255" s="1"/>
+    </row>
+    <row r="1256" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1256" s="1"/>
+    </row>
+    <row r="1257" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1257" s="1"/>
+    </row>
+    <row r="1258" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1258" s="1"/>
+    </row>
+    <row r="1259" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1259" s="1"/>
+    </row>
+    <row r="1260" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1260" s="1"/>
+    </row>
+    <row r="1261" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1261" s="1"/>
+    </row>
+    <row r="1262" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1262" s="1"/>
+    </row>
+    <row r="1263" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1263" s="1"/>
+    </row>
+    <row r="1264" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1264" s="1"/>
+    </row>
+    <row r="1265" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1265" s="1"/>
+    </row>
+    <row r="1266" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1266" s="1"/>
+    </row>
+    <row r="1267" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1267" s="1"/>
+    </row>
+    <row r="1268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1268" s="1"/>
+    </row>
+    <row r="1269" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1269" s="1"/>
+    </row>
+    <row r="1270" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1270" s="1"/>
+    </row>
+    <row r="1271" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1271" s="1"/>
+    </row>
+    <row r="1272" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1272" s="1"/>
+    </row>
+    <row r="1273" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1273" s="3"/>
+    </row>
+    <row r="1274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1274" s="1"/>
+    </row>
+    <row r="1275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1275" s="1"/>
+    </row>
+    <row r="1276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1276" s="1"/>
+    </row>
+    <row r="1277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1277" s="1"/>
+    </row>
+    <row r="1278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1278" s="1"/>
+    </row>
+    <row r="1279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1279" s="1"/>
+    </row>
+    <row r="1280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1280" s="1"/>
+    </row>
+    <row r="1281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1281" s="1"/>
+    </row>
+    <row r="1282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1282" s="1"/>
+    </row>
+    <row r="1283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1283" s="1"/>
+    </row>
+    <row r="1284" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1284" s="1"/>
+    </row>
+    <row r="1285" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1285" s="1"/>
+    </row>
+    <row r="1286" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1286" s="1"/>
+    </row>
+    <row r="1287" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1287" s="1"/>
+    </row>
+    <row r="1288" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1288" s="1"/>
+    </row>
+    <row r="1289" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1289" s="1"/>
+    </row>
+    <row r="1290" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1290" s="1"/>
+    </row>
+    <row r="1291" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1291" s="1"/>
+    </row>
+    <row r="1292" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1292" s="1"/>
+    </row>
+    <row r="1293" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1293" s="1"/>
+    </row>
+    <row r="1294" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1294" s="1"/>
+    </row>
+    <row r="1295" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1295" s="1"/>
+    </row>
+    <row r="1296" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1296" s="1"/>
+    </row>
+    <row r="1297" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1297" s="1"/>
+    </row>
+    <row r="1298" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1298" s="1"/>
+    </row>
+    <row r="1299" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1299" s="1"/>
+    </row>
+    <row r="1300" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1300" s="1"/>
+    </row>
+    <row r="1301" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1301" s="1"/>
+    </row>
+    <row r="1302" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1302" s="1"/>
+    </row>
+    <row r="1303" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1303" s="1"/>
+    </row>
+    <row r="1304" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1304" s="1"/>
+    </row>
+    <row r="1305" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1305" s="1"/>
+    </row>
+    <row r="1306" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1306" s="1"/>
+    </row>
+    <row r="1307" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1307" s="1"/>
+    </row>
+    <row r="1308" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1308" s="1"/>
+    </row>
+    <row r="1309" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1309" s="1"/>
+    </row>
+    <row r="1310" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1310" s="1"/>
+    </row>
+    <row r="1311" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1311" s="1"/>
+    </row>
+    <row r="1312" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1312" s="1"/>
+    </row>
+    <row r="1313" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1313" s="3"/>
+    </row>
+    <row r="1314" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1314" s="1"/>
+    </row>
+    <row r="1315" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1315" s="1"/>
+    </row>
+    <row r="1316" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1316" s="1"/>
+    </row>
+    <row r="1317" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1317" s="1"/>
+    </row>
+    <row r="1318" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1318" s="1"/>
+    </row>
+    <row r="1319" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1319" s="1"/>
+    </row>
+    <row r="1320" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1320" s="1"/>
+    </row>
+    <row r="1321" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1321" s="1"/>
+    </row>
+    <row r="1322" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1322" s="1"/>
+    </row>
+    <row r="1323" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1323" s="1"/>
+    </row>
+    <row r="1324" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1324" s="1"/>
+    </row>
+    <row r="1325" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1325" s="1"/>
+    </row>
+    <row r="1326" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1326" s="1"/>
+    </row>
+    <row r="1327" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1327" s="1"/>
+    </row>
+    <row r="1328" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1328" s="1"/>
+    </row>
+    <row r="1329" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1329" s="1"/>
+    </row>
+    <row r="1330" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1330" s="1"/>
+    </row>
+    <row r="1331" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1331" s="1"/>
+    </row>
+    <row r="1332" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1332" s="1"/>
+    </row>
+    <row r="1333" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1333" s="1"/>
+    </row>
+    <row r="1334" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1334" s="1"/>
+    </row>
+    <row r="1335" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1335" s="1"/>
+    </row>
+    <row r="1336" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1336" s="1"/>
+    </row>
+    <row r="1337" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1337" s="1"/>
+    </row>
+    <row r="1338" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1338" s="1"/>
+    </row>
+    <row r="1339" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1339" s="1"/>
+    </row>
+    <row r="1340" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1340" s="1"/>
+    </row>
+    <row r="1341" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1341" s="1"/>
+    </row>
+    <row r="1342" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1342" s="1"/>
+    </row>
+    <row r="1343" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1343" s="1"/>
+    </row>
+    <row r="1344" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1344" s="1"/>
+    </row>
+    <row r="1345" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1345" s="1"/>
+    </row>
+    <row r="1346" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1346" s="1"/>
+    </row>
+    <row r="1347" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1347" s="1"/>
+    </row>
+    <row r="1348" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1348" s="1"/>
+    </row>
+    <row r="1349" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1349" s="1"/>
+    </row>
+    <row r="1350" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1350" s="1"/>
+    </row>
+    <row r="1351" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1351" s="1"/>
+    </row>
+    <row r="1352" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1352" s="1"/>
+    </row>
+    <row r="1353" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1353" s="1"/>
+    </row>
+    <row r="1354" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1354" s="1"/>
+    </row>
+    <row r="1355" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1355" s="1"/>
+    </row>
+    <row r="1356" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1356" s="1"/>
+    </row>
+    <row r="1357" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1357" s="1"/>
+    </row>
+    <row r="1358" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1358" s="1"/>
+    </row>
+    <row r="1359" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1359" s="1"/>
+    </row>
+    <row r="1360" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1360" s="1"/>
+    </row>
+    <row r="1361" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1361" s="1"/>
+    </row>
+    <row r="1362" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1362" s="1"/>
+    </row>
+    <row r="1363" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1363" s="1"/>
+    </row>
+    <row r="1364" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1364" s="1"/>
+    </row>
+    <row r="1365" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1365" s="1"/>
+    </row>
+    <row r="1366" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1366" s="1"/>
+    </row>
+    <row r="1367" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1367" s="1"/>
+    </row>
+    <row r="1368" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1368" s="1"/>
+    </row>
+    <row r="1369" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1369" s="1"/>
+    </row>
+    <row r="1370" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1370" s="1"/>
+    </row>
+    <row r="1371" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1371" s="1"/>
+    </row>
+    <row r="1372" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1372" s="1"/>
+    </row>
+    <row r="1373" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1373" s="1"/>
+    </row>
+    <row r="1374" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1374" s="1"/>
+    </row>
+    <row r="1375" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1375" s="1"/>
+    </row>
+    <row r="1376" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1376" s="1"/>
+    </row>
+    <row r="1377" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1377" s="1"/>
+    </row>
+    <row r="1378" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1378" s="1"/>
+    </row>
+    <row r="1379" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1379" s="1"/>
+    </row>
+    <row r="1380" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1380" s="1"/>
+    </row>
+    <row r="1381" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1381" s="1"/>
+    </row>
+    <row r="1382" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1382" s="1"/>
+    </row>
+    <row r="1383" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1383" s="1"/>
+    </row>
+    <row r="1384" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1384" s="1"/>
+    </row>
+    <row r="1385" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1385" s="1"/>
+    </row>
+    <row r="1386" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1386" s="1"/>
+    </row>
+    <row r="1387" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1387" s="1"/>
+    </row>
+    <row r="1388" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1388" s="1"/>
+    </row>
+    <row r="1389" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1389" s="1"/>
+    </row>
+    <row r="1390" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1390" s="1"/>
+    </row>
+    <row r="1391" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1391" s="1"/>
+    </row>
+    <row r="1392" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1392" s="1"/>
+    </row>
+    <row r="1393" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1393" s="1"/>
+    </row>
+    <row r="1394" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1394" s="1"/>
+    </row>
+    <row r="1395" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1395" s="1"/>
+    </row>
+    <row r="1396" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1396" s="1"/>
+    </row>
+    <row r="1397" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1397" s="1"/>
+    </row>
+    <row r="1398" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1398" s="1"/>
+    </row>
+    <row r="1399" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1399" s="1"/>
+    </row>
+    <row r="1400" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1400" s="1"/>
+    </row>
+    <row r="1401" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1401" s="1"/>
+    </row>
+    <row r="1402" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1402" s="1"/>
+    </row>
+    <row r="1403" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1403" s="1"/>
+    </row>
+    <row r="1404" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1404" s="1"/>
+    </row>
+    <row r="1405" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1405" s="1"/>
+    </row>
+    <row r="1406" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1406" s="1"/>
+    </row>
+    <row r="1407" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1407" s="1"/>
+    </row>
+    <row r="1408" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1408" s="1"/>
+    </row>
+    <row r="1409" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1409" s="1"/>
+    </row>
+    <row r="1410" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1410" s="1"/>
+    </row>
+    <row r="1411" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1411" s="1"/>
+    </row>
+    <row r="1412" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1412" s="1"/>
+    </row>
+    <row r="1413" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1413" s="1"/>
+    </row>
+    <row r="1414" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1414" s="1"/>
+    </row>
+    <row r="1415" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1415" s="1"/>
+    </row>
+    <row r="1416" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1416" s="1"/>
+    </row>
+    <row r="1417" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1417" s="1"/>
+    </row>
+    <row r="1418" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1418" s="1"/>
+    </row>
+    <row r="1419" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1419" s="1"/>
+    </row>
+    <row r="1420" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1420" s="1"/>
+    </row>
+    <row r="1421" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1421" s="1"/>
+    </row>
+    <row r="1422" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1422" s="1"/>
+    </row>
+    <row r="1423" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1423" s="1"/>
+    </row>
+    <row r="1424" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1424" s="1"/>
+    </row>
+    <row r="1425" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1425" s="1"/>
+    </row>
+    <row r="1426" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1426" s="1"/>
+    </row>
+    <row r="1427" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1427" s="1"/>
+    </row>
+    <row r="1428" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1428" s="1"/>
+    </row>
+    <row r="1429" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1429" s="1"/>
+    </row>
+    <row r="1430" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1430" s="1"/>
+    </row>
+    <row r="1431" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1431" s="1"/>
+    </row>
+    <row r="1432" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1432" s="1"/>
+    </row>
+    <row r="1433" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1433" s="1"/>
+    </row>
+    <row r="1434" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1434" s="1"/>
+    </row>
+    <row r="1435" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1435" s="1"/>
+    </row>
+    <row r="1436" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1436" s="1"/>
+    </row>
+    <row r="1437" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1437" s="1"/>
+    </row>
+    <row r="1438" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1438" s="1"/>
+    </row>
+    <row r="1439" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1439" s="1"/>
+    </row>
+    <row r="1440" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1440" s="1"/>
+    </row>
+    <row r="1441" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1441" s="1"/>
+    </row>
+    <row r="1442" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1442" s="1"/>
+    </row>
+    <row r="1443" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1443" s="1"/>
+    </row>
+    <row r="1444" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1444" s="1"/>
+    </row>
+    <row r="1445" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1445" s="1"/>
+    </row>
+    <row r="1446" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1446" s="1"/>
+    </row>
+    <row r="1447" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1447" s="1"/>
+    </row>
+    <row r="1448" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1448" s="1"/>
+    </row>
+    <row r="1449" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1449" s="1"/>
+    </row>
+    <row r="1450" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1450" s="1"/>
+    </row>
+    <row r="1451" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1451" s="1"/>
+    </row>
+    <row r="1452" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1452" s="1"/>
+    </row>
+    <row r="1453" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1453" s="1"/>
+    </row>
+    <row r="1454" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1454" s="1"/>
+    </row>
+    <row r="1455" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1455" s="1"/>
+    </row>
+    <row r="1456" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1456" s="1"/>
+    </row>
+    <row r="1457" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1457" s="1"/>
+    </row>
+    <row r="1458" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1458" s="1"/>
+    </row>
+    <row r="1459" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1459" s="1"/>
+    </row>
+    <row r="1460" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1460" s="1"/>
+    </row>
+    <row r="1461" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1461" s="1"/>
+    </row>
+    <row r="1462" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1462" s="1"/>
+    </row>
+    <row r="1463" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1463" s="1"/>
+    </row>
+    <row r="1464" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1464" s="1"/>
+    </row>
+    <row r="1465" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1465" s="1"/>
+    </row>
+    <row r="1466" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1466" s="1"/>
+    </row>
+    <row r="1467" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1467" s="1"/>
+    </row>
+    <row r="1468" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1468" s="1"/>
+    </row>
+    <row r="1469" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1469" s="1"/>
+    </row>
+    <row r="1470" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1470" s="1"/>
+    </row>
+    <row r="1471" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1471" s="1"/>
+    </row>
+    <row r="1472" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1472" s="1"/>
+    </row>
+    <row r="1473" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1473" s="1"/>
+    </row>
+    <row r="1474" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1474" s="1"/>
+    </row>
+    <row r="1475" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1475" s="1"/>
+    </row>
+    <row r="1476" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1476" s="1"/>
+    </row>
+    <row r="1477" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1477" s="1"/>
+    </row>
+    <row r="1478" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1478" s="1"/>
+    </row>
+    <row r="1479" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1479" s="1"/>
+    </row>
+    <row r="1480" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1480" s="1"/>
+    </row>
+    <row r="1481" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1481" s="1"/>
+    </row>
+    <row r="1482" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1482" s="1"/>
+    </row>
+    <row r="1483" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1483" s="1"/>
+    </row>
+    <row r="1484" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1484" s="1"/>
+    </row>
+    <row r="1485" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1485" s="1"/>
+    </row>
+    <row r="1486" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1486" s="1"/>
+    </row>
+    <row r="1487" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1487" s="1"/>
+    </row>
+    <row r="1488" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1488" s="1"/>
+    </row>
+    <row r="1489" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1489" s="1"/>
+    </row>
+    <row r="1490" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1490" s="1"/>
+    </row>
+    <row r="1491" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1491" s="1"/>
+    </row>
+    <row r="1492" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1492" s="1"/>
+    </row>
+    <row r="1493" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1493" s="1"/>
+    </row>
+    <row r="1494" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1494" s="1"/>
+    </row>
+    <row r="1495" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1495" s="1"/>
+    </row>
+    <row r="1496" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1496" s="1"/>
+    </row>
+    <row r="1497" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1497" s="1"/>
+    </row>
+    <row r="1498" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1498" s="1"/>
+    </row>
+    <row r="1499" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1499" s="1"/>
+    </row>
+    <row r="1500" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1500" s="1"/>
+    </row>
+    <row r="1501" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1501" s="1"/>
+    </row>
+    <row r="1502" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1502" s="1"/>
+    </row>
+    <row r="1503" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1503" s="1"/>
+    </row>
+    <row r="1504" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1504" s="1"/>
+    </row>
+    <row r="1505" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1505" s="1"/>
+    </row>
+    <row r="1506" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1506" s="1"/>
+    </row>
+    <row r="1507" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1507" s="1"/>
+    </row>
+    <row r="1508" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1508" s="1"/>
+    </row>
+    <row r="1509" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1509" s="1"/>
+    </row>
+    <row r="1510" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1510" s="1"/>
+    </row>
+    <row r="1511" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1511" s="1"/>
+    </row>
+    <row r="1512" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1512" s="1"/>
+    </row>
+    <row r="1513" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1513" s="1"/>
+    </row>
+    <row r="1514" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1514" s="1"/>
+    </row>
+    <row r="1515" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1515" s="1"/>
+    </row>
+    <row r="1516" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1516" s="1"/>
+    </row>
+    <row r="1517" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1517" s="1"/>
+    </row>
+    <row r="1518" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1518" s="1"/>
+    </row>
+    <row r="1519" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1519" s="1"/>
+    </row>
+    <row r="1520" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1520" s="1"/>
+    </row>
+    <row r="1521" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1521" s="1"/>
+    </row>
+    <row r="1522" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1522" s="1"/>
+    </row>
+    <row r="1523" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1523" s="1"/>
+    </row>
+    <row r="1524" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1524" s="1"/>
+    </row>
+    <row r="1525" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1525" s="1"/>
+    </row>
+    <row r="1526" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1526" s="1"/>
+    </row>
+    <row r="1527" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1527" s="1"/>
+    </row>
+    <row r="1528" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1528" s="1"/>
+    </row>
+    <row r="1529" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1529" s="1"/>
+    </row>
+    <row r="1530" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1530" s="1"/>
+    </row>
+    <row r="1531" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1531" s="1"/>
+    </row>
+    <row r="1532" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1532" s="1"/>
+    </row>
+    <row r="1533" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1533" s="1"/>
+    </row>
+    <row r="1534" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1534" s="1"/>
+    </row>
+    <row r="1535" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1535" s="1"/>
+    </row>
+    <row r="1536" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1536" s="1"/>
+    </row>
+    <row r="1537" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1537" s="1"/>
+    </row>
+    <row r="1538" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1538" s="1"/>
+    </row>
+    <row r="1539" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1539" s="1"/>
+    </row>
+    <row r="1540" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1540" s="1"/>
+    </row>
+    <row r="1541" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1541" s="1"/>
+    </row>
+    <row r="1542" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1542" s="1"/>
+    </row>
+    <row r="1543" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1543" s="1"/>
+    </row>
+    <row r="1544" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1544" s="1"/>
+    </row>
+    <row r="1545" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1545" s="1"/>
+    </row>
+    <row r="1546" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1546" s="1"/>
+    </row>
+    <row r="1547" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1547" s="1"/>
+    </row>
+    <row r="1548" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1548" s="1"/>
+    </row>
+    <row r="1549" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1549" s="1"/>
+    </row>
+    <row r="1550" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1550" s="1"/>
+    </row>
+    <row r="1551" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1551" s="1"/>
+    </row>
+    <row r="1552" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1552" s="1"/>
+    </row>
+    <row r="1553" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1553" s="1"/>
+    </row>
+    <row r="1554" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1554" s="1"/>
+    </row>
+    <row r="1555" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1555" s="1"/>
+    </row>
+    <row r="1556" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1556" s="1"/>
+    </row>
+    <row r="1557" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1557" s="1"/>
+    </row>
+    <row r="1558" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1558" s="1"/>
+    </row>
+    <row r="1559" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1559" s="1"/>
+    </row>
+    <row r="1560" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1560" s="1"/>
+    </row>
+    <row r="1561" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1561" s="1"/>
+    </row>
+    <row r="1562" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1562" s="1"/>
+    </row>
+    <row r="1563" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1563" s="1"/>
+    </row>
+    <row r="1564" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1564" s="1"/>
+    </row>
+    <row r="1565" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1565" s="1"/>
+    </row>
+    <row r="1566" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1566" s="1"/>
+    </row>
+    <row r="1567" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1567" s="1"/>
+    </row>
+    <row r="1568" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1568" s="1"/>
+    </row>
+    <row r="1569" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1569" s="1"/>
+    </row>
+    <row r="1570" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1570" s="1"/>
+    </row>
+    <row r="1571" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1571" s="1"/>
+    </row>
+    <row r="1572" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1572" s="1"/>
+    </row>
+    <row r="1573" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1573" s="1"/>
+    </row>
+    <row r="1574" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1574" s="1"/>
+    </row>
+    <row r="1575" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1575" s="1"/>
+    </row>
+    <row r="1576" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1576" s="1"/>
+    </row>
+    <row r="1577" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1577" s="1"/>
+    </row>
+    <row r="1578" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1578" s="1"/>
+    </row>
+    <row r="1579" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1579" s="1"/>
+    </row>
+    <row r="1580" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1580" s="1"/>
+    </row>
+    <row r="1581" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1581" s="1"/>
+    </row>
+    <row r="1582" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1582" s="1"/>
+    </row>
+    <row r="1583" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1583" s="1"/>
+    </row>
+    <row r="1584" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1584" s="1"/>
+    </row>
+    <row r="1585" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1585" s="1"/>
+    </row>
+    <row r="1586" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1586" s="1"/>
+    </row>
+    <row r="1587" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1587" s="1"/>
+    </row>
+    <row r="1588" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1588" s="1"/>
+    </row>
+    <row r="1589" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1589" s="1"/>
+    </row>
+    <row r="1590" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1590" s="1"/>
+    </row>
+    <row r="1591" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1591" s="1"/>
+    </row>
+    <row r="1592" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1592" s="1"/>
+    </row>
+    <row r="1593" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1593" s="1"/>
+    </row>
+    <row r="1594" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1594" s="1"/>
+    </row>
+    <row r="1595" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1595" s="1"/>
+    </row>
+    <row r="1596" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1596" s="1"/>
+    </row>
+    <row r="1597" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1597" s="1"/>
+    </row>
+    <row r="1598" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1598" s="1"/>
+    </row>
+    <row r="1599" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1599" s="1"/>
+    </row>
+    <row r="1600" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1600" s="1"/>
+    </row>
+    <row r="1601" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1601" s="1"/>
+    </row>
+    <row r="1602" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1602" s="1"/>
+    </row>
+    <row r="1603" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1603" s="1"/>
+    </row>
+    <row r="1604" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1604" s="1"/>
+    </row>
+    <row r="1605" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1605" s="1"/>
+    </row>
+    <row r="1606" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1606" s="1"/>
+    </row>
+    <row r="1607" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1607" s="1"/>
+    </row>
+    <row r="1608" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1608" s="1"/>
+    </row>
+    <row r="1609" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1609" s="1"/>
+    </row>
+    <row r="1610" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1610" s="1"/>
+    </row>
+    <row r="1611" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1611" s="1"/>
+    </row>
+    <row r="1612" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1612" s="3"/>
+    </row>
+    <row r="1613" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1613" s="1"/>
+    </row>
+    <row r="1614" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1614" s="1"/>
+    </row>
+    <row r="1615" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1615" s="1"/>
+    </row>
+    <row r="1616" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1616" s="1"/>
+    </row>
+    <row r="1617" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1617" s="1"/>
+    </row>
+    <row r="1618" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1618" s="1"/>
+    </row>
+    <row r="1619" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1619" s="1"/>
+    </row>
+    <row r="1620" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1620" s="1"/>
+    </row>
+    <row r="1621" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1621" s="1"/>
+    </row>
+    <row r="1622" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1622" s="1"/>
+    </row>
+    <row r="1623" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1623" s="1"/>
+    </row>
+    <row r="1624" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1624" s="1"/>
+    </row>
+    <row r="1625" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1625" s="1"/>
+    </row>
+    <row r="1626" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1626" s="1"/>
+    </row>
+    <row r="1627" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1627" s="1"/>
+    </row>
+    <row r="1628" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1628" s="1"/>
+    </row>
+    <row r="1629" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1629" s="1"/>
+    </row>
+    <row r="1630" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1630" s="1"/>
+    </row>
+    <row r="1631" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1631" s="1"/>
+    </row>
+    <row r="1632" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1632" s="1"/>
+    </row>
+    <row r="1633" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1633" s="1"/>
+    </row>
+    <row r="1634" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1634" s="1"/>
+    </row>
+    <row r="1635" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1635" s="1"/>
+    </row>
+    <row r="1636" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1636" s="1"/>
+    </row>
+    <row r="1637" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1637" s="1"/>
+    </row>
+    <row r="1638" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1638" s="1"/>
+    </row>
+    <row r="1639" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1639" s="1"/>
+    </row>
+    <row r="1640" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1640" s="1"/>
+    </row>
+    <row r="1641" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1641" s="1"/>
+    </row>
+    <row r="1642" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1642" s="1"/>
+    </row>
+    <row r="1643" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1643" s="1"/>
+    </row>
+    <row r="1644" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1644" s="1"/>
+    </row>
+    <row r="1645" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1645" s="1"/>
+    </row>
+    <row r="1646" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1646" s="1"/>
+    </row>
+    <row r="1647" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1647" s="1"/>
+    </row>
+    <row r="1648" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1648" s="1"/>
+    </row>
+    <row r="1649" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1649" s="1"/>
+    </row>
+    <row r="1650" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1650" s="1"/>
+    </row>
+    <row r="1651" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1651" s="1"/>
+    </row>
+    <row r="1652" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1652" s="1"/>
+    </row>
+    <row r="1653" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1653" s="1"/>
+    </row>
+    <row r="1654" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1654" s="1"/>
+    </row>
+    <row r="1655" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1655" s="1"/>
+    </row>
+    <row r="1656" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1656" s="1"/>
+    </row>
+    <row r="1657" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1657" s="1"/>
+    </row>
+    <row r="1658" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1658" s="1"/>
+    </row>
+    <row r="1659" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1659" s="1"/>
+    </row>
+    <row r="1660" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1660" s="1"/>
+    </row>
+    <row r="1661" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1661" s="1"/>
+    </row>
+    <row r="1662" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1662" s="1"/>
+    </row>
+    <row r="1663" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1663" s="1"/>
+    </row>
+    <row r="1664" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1664" s="1"/>
+    </row>
+    <row r="1665" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1665" s="1"/>
+    </row>
+    <row r="1666" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1666" s="1"/>
+    </row>
+    <row r="1667" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1667" s="1"/>
+    </row>
+    <row r="1668" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1668" s="1"/>
+    </row>
+    <row r="1669" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1669" s="1"/>
+    </row>
+    <row r="1670" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1670" s="1"/>
+    </row>
+    <row r="1671" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1671" s="1"/>
+    </row>
+    <row r="1672" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1672" s="1"/>
+    </row>
+    <row r="1673" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1673" s="1"/>
+    </row>
+    <row r="1674" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1674" s="1"/>
+    </row>
+    <row r="1675" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1675" s="1"/>
+    </row>
+    <row r="1676" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1676" s="1"/>
+    </row>
+    <row r="1677" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1677" s="1"/>
+    </row>
+    <row r="1678" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1678" s="1"/>
+    </row>
+    <row r="1679" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1679" s="1"/>
+    </row>
+    <row r="1680" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1680" s="1"/>
+    </row>
+    <row r="1681" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1681" s="1"/>
+    </row>
+    <row r="1682" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1682" s="1"/>
+    </row>
+    <row r="1683" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1683" s="1"/>
+    </row>
+    <row r="1684" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1684" s="1"/>
+    </row>
+    <row r="1685" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1685" s="1"/>
+    </row>
+    <row r="1686" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1686" s="1"/>
+    </row>
+    <row r="1687" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1687" s="1"/>
+    </row>
+    <row r="1688" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1688" s="1"/>
+    </row>
+    <row r="1689" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1689" s="1"/>
+    </row>
+    <row r="1690" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1690" s="1"/>
+    </row>
+    <row r="1691" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1691" s="1"/>
+    </row>
+    <row r="1692" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1692" s="1"/>
+    </row>
+    <row r="1693" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1693" s="1"/>
+    </row>
+    <row r="1694" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1694" s="1"/>
+    </row>
+    <row r="1695" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1695" s="1"/>
+    </row>
+    <row r="1696" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1696" s="1"/>
+    </row>
+    <row r="1697" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1697" s="1"/>
+    </row>
+    <row r="1698" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1698" s="1"/>
+    </row>
+    <row r="1699" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1699" s="1"/>
+    </row>
+    <row r="1700" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1700" s="1"/>
+    </row>
+    <row r="1701" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1701" s="1"/>
+    </row>
+    <row r="1702" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1702" s="1"/>
+    </row>
+    <row r="1703" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1703" s="1"/>
+    </row>
+    <row r="1704" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1704" s="1"/>
+    </row>
+    <row r="1705" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1705" s="1"/>
+    </row>
+    <row r="1706" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1706" s="1"/>
+    </row>
+    <row r="1707" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1707" s="1"/>
+    </row>
+    <row r="1708" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1708" s="1"/>
+    </row>
+    <row r="1709" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1709" s="1"/>
+    </row>
+    <row r="1710" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1710" s="1"/>
+    </row>
+    <row r="1711" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1711" s="1"/>
+    </row>
+    <row r="1712" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1712" s="1"/>
+    </row>
+    <row r="1713" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1713" s="1"/>
+    </row>
+    <row r="1714" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1714" s="1"/>
+    </row>
+    <row r="1715" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1715" s="1"/>
+    </row>
+    <row r="1716" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1716" s="1"/>
+    </row>
+    <row r="1717" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1717" s="1"/>
+    </row>
+    <row r="1718" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1718" s="1"/>
+    </row>
+    <row r="1719" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1719" s="1"/>
+    </row>
+    <row r="1720" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1720" s="1"/>
+    </row>
+    <row r="1721" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1721" s="1"/>
+    </row>
+    <row r="1722" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1722" s="1"/>
+    </row>
+    <row r="1723" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1723" s="1"/>
+    </row>
+    <row r="1724" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1724" s="1"/>
+    </row>
+    <row r="1725" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1725" s="1"/>
+    </row>
+    <row r="1726" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1726" s="1"/>
+    </row>
+    <row r="1727" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1727" s="1"/>
+    </row>
+    <row r="1728" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1728" s="1"/>
+    </row>
+    <row r="1729" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1729" s="1"/>
+    </row>
+    <row r="1730" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1730" s="1"/>
+    </row>
+    <row r="1731" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1731" s="1"/>
+    </row>
+    <row r="1732" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1732" s="1"/>
+    </row>
+    <row r="1733" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1733" s="1"/>
+    </row>
+    <row r="1734" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1734" s="1"/>
+    </row>
+    <row r="1735" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1735" s="1"/>
+    </row>
+    <row r="1736" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1736" s="1"/>
+    </row>
+    <row r="1737" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1737" s="1"/>
+    </row>
+    <row r="1738" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1738" s="1"/>
+    </row>
+    <row r="1739" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1739" s="1"/>
+    </row>
+    <row r="1740" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1740" s="1"/>
+    </row>
+    <row r="1741" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1741" s="1"/>
+    </row>
+    <row r="1742" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1742" s="1"/>
+    </row>
+    <row r="1743" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1743" s="1"/>
+    </row>
+    <row r="1744" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1744" s="1"/>
+    </row>
+    <row r="1745" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1745" s="1"/>
+    </row>
+    <row r="1746" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1746" s="1"/>
+    </row>
+    <row r="1747" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1747" s="1"/>
+    </row>
+    <row r="1748" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1748" s="1"/>
+    </row>
+    <row r="1749" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1749" s="1"/>
+    </row>
+    <row r="1750" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1750" s="1"/>
+    </row>
+    <row r="1751" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1751" s="1"/>
+    </row>
+    <row r="1752" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1752" s="1"/>
+    </row>
+    <row r="1753" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1753" s="1"/>
+    </row>
+    <row r="1754" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1754" s="1"/>
+    </row>
+    <row r="1755" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1755" s="1"/>
+    </row>
+    <row r="1756" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1756" s="1"/>
+    </row>
+    <row r="1757" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1757" s="1"/>
+    </row>
+    <row r="1758" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1758" s="1"/>
+    </row>
+    <row r="1759" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1759" s="1"/>
+    </row>
+    <row r="1760" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1760" s="1"/>
+    </row>
+    <row r="1761" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1761" s="1"/>
+    </row>
+    <row r="1762" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1762" s="1"/>
+    </row>
+    <row r="1763" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1763" s="1"/>
+    </row>
+    <row r="1764" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1764" s="3"/>
+    </row>
+    <row r="1765" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1765" s="1"/>
+    </row>
+    <row r="1766" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1766" s="1"/>
+    </row>
+    <row r="1767" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1767" s="1"/>
+    </row>
+    <row r="1768" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1768" s="1"/>
+    </row>
+    <row r="1769" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1769" s="1"/>
+    </row>
+    <row r="1770" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1770" s="1"/>
+    </row>
+    <row r="1771" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1771" s="1"/>
+    </row>
+    <row r="1772" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1772" s="1"/>
+    </row>
+    <row r="1773" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1773" s="1"/>
+    </row>
+    <row r="1774" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1774" s="1"/>
+    </row>
+    <row r="1775" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1775" s="1"/>
+    </row>
+    <row r="1776" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1776" s="1"/>
+    </row>
+    <row r="1777" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1777" s="1"/>
+    </row>
+    <row r="1778" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1778" s="1"/>
+    </row>
+    <row r="1779" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1779" s="1"/>
+    </row>
+    <row r="1780" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1780" s="1"/>
+    </row>
+    <row r="1781" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1781" s="1"/>
+    </row>
+    <row r="1782" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1782" s="1"/>
+    </row>
+    <row r="1783" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1783" s="1"/>
+    </row>
+    <row r="1784" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1784" s="1"/>
+    </row>
+    <row r="1785" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1785" s="1"/>
+    </row>
+    <row r="1786" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1786" s="1"/>
+    </row>
+    <row r="1787" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1787" s="1"/>
+    </row>
+    <row r="1788" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1788" s="1"/>
+    </row>
+    <row r="1789" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1789" s="1"/>
+    </row>
+    <row r="1790" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1790" s="1"/>
+    </row>
+    <row r="1791" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1791" s="1"/>
+    </row>
+    <row r="1792" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1792" s="1"/>
+    </row>
+    <row r="1793" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1793" s="1"/>
+    </row>
+    <row r="1794" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1794" s="1"/>
+    </row>
+    <row r="1795" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1795" s="1"/>
+    </row>
+    <row r="1796" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1796" s="1"/>
+    </row>
+    <row r="1797" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1797" s="1"/>
+    </row>
+    <row r="1798" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1798" s="1"/>
+    </row>
+    <row r="1799" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1799" s="1"/>
+    </row>
+    <row r="1800" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1800" s="1"/>
+    </row>
+    <row r="1801" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1801" s="1"/>
+    </row>
+    <row r="1802" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1802" s="1"/>
+    </row>
+    <row r="1803" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1803" s="1"/>
+    </row>
+    <row r="1804" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1804" s="1"/>
+    </row>
+    <row r="1805" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1805" s="1"/>
+    </row>
+    <row r="1806" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1806" s="1"/>
+    </row>
+    <row r="1807" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1807" s="1"/>
+    </row>
+    <row r="1808" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1808" s="1"/>
+    </row>
+    <row r="1809" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1809" s="1"/>
+    </row>
+    <row r="1810" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1810" s="1"/>
+    </row>
+    <row r="1811" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1811" s="1"/>
+    </row>
+    <row r="1812" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1812" s="1"/>
+    </row>
+    <row r="1813" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1813" s="1"/>
+    </row>
+    <row r="1814" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1814" s="1"/>
+    </row>
+    <row r="1815" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1815" s="1"/>
+    </row>
+    <row r="1816" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1816" s="1"/>
+    </row>
+    <row r="1817" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1817" s="1"/>
+    </row>
+    <row r="1818" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1818" s="1"/>
+    </row>
+    <row r="1819" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1819" s="1"/>
+    </row>
+    <row r="1820" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1820" s="1"/>
+    </row>
+    <row r="1821" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1821" s="1"/>
+    </row>
+    <row r="1822" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1822" s="1"/>
+    </row>
+    <row r="1823" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1823" s="1"/>
+    </row>
+    <row r="1824" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1824" s="1"/>
+    </row>
+    <row r="1825" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1825" s="1"/>
+    </row>
+    <row r="1826" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1826" s="1"/>
+    </row>
+    <row r="1827" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1827" s="1"/>
+    </row>
+    <row r="1828" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1828" s="1"/>
+    </row>
+    <row r="1829" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1829" s="1"/>
+    </row>
+    <row r="1830" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1830" s="1"/>
+    </row>
+    <row r="1831" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1831" s="1"/>
+    </row>
+    <row r="1832" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1832" s="1"/>
+    </row>
+    <row r="1833" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1833" s="1"/>
+    </row>
+    <row r="1834" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1834" s="1"/>
+    </row>
+    <row r="1835" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1835" s="1"/>
+    </row>
+    <row r="1836" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1836" s="1"/>
+    </row>
+    <row r="1837" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1837" s="1"/>
+    </row>
+    <row r="1838" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1838" s="1"/>
+    </row>
+    <row r="1839" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1839" s="1"/>
+    </row>
+    <row r="1840" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1840" s="1"/>
+    </row>
+    <row r="1841" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1841" s="1"/>
+    </row>
+    <row r="1842" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1842" s="1"/>
+    </row>
+    <row r="1843" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1843" s="1"/>
+    </row>
+    <row r="1844" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1844" s="1"/>
+    </row>
+    <row r="1845" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1845" s="1"/>
+    </row>
+    <row r="1846" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1846" s="1"/>
+    </row>
+    <row r="1847" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1847" s="1"/>
+    </row>
+    <row r="1848" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1848" s="1"/>
+    </row>
+    <row r="1849" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1849" s="1"/>
+    </row>
+    <row r="1850" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1850" s="1"/>
+    </row>
+    <row r="1851" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1851" s="1"/>
+    </row>
+    <row r="1852" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1852" s="1"/>
+    </row>
+    <row r="1853" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1853" s="1"/>
+    </row>
+    <row r="1854" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1854" s="1"/>
+    </row>
+    <row r="1855" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1855" s="1"/>
+    </row>
+    <row r="1856" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1856" s="1"/>
+    </row>
+    <row r="1857" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1857" s="1"/>
+    </row>
+    <row r="1858" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1858" s="1"/>
+    </row>
+    <row r="1859" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1859" s="1"/>
+    </row>
+    <row r="1860" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1860" s="1"/>
+    </row>
+    <row r="1861" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1861" s="1"/>
+    </row>
+    <row r="1862" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1862" s="1"/>
+    </row>
+    <row r="1863" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1863" s="1"/>
+    </row>
+    <row r="1864" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1864" s="1"/>
+    </row>
+    <row r="1865" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1865" s="1"/>
+    </row>
+    <row r="1866" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1866" s="1"/>
+    </row>
+    <row r="1867" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1867" s="1"/>
+    </row>
+    <row r="1868" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1868" s="1"/>
+    </row>
+    <row r="1869" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1869" s="1"/>
+    </row>
+    <row r="1870" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1870" s="1"/>
+    </row>
+    <row r="1871" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1871" s="1"/>
+    </row>
+    <row r="1872" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1872" s="1"/>
+    </row>
+    <row r="1873" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1873" s="1"/>
+    </row>
+    <row r="1874" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1874" s="1"/>
+    </row>
+    <row r="1875" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1875" s="1"/>
+    </row>
+    <row r="1876" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1876" s="1"/>
+    </row>
+    <row r="1877" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1877" s="1"/>
+    </row>
+    <row r="1878" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1878" s="1"/>
+    </row>
+    <row r="1879" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1879" s="1"/>
+    </row>
+    <row r="1880" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1880" s="1"/>
+    </row>
+    <row r="1881" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1881" s="1"/>
+    </row>
+    <row r="1882" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1882" s="1"/>
+    </row>
+    <row r="1883" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1883" s="1"/>
+    </row>
+    <row r="1884" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1884" s="1"/>
+    </row>
+    <row r="1885" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1885" s="1"/>
+    </row>
+    <row r="1886" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1886" s="1"/>
+    </row>
+    <row r="1887" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1887" s="1"/>
+    </row>
+    <row r="1888" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1888" s="1"/>
+    </row>
+    <row r="1889" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1889" s="1"/>
+    </row>
+    <row r="1890" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1890" s="1"/>
+    </row>
+    <row r="1891" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1891" s="1"/>
+    </row>
+    <row r="1892" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1892" s="1"/>
+    </row>
+    <row r="1893" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1893" s="1"/>
+    </row>
+    <row r="1894" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1894" s="3"/>
+    </row>
+    <row r="1895" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1895" s="1"/>
+    </row>
+    <row r="1896" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1896" s="1"/>
+    </row>
+    <row r="1897" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1897" s="1"/>
+    </row>
+    <row r="1898" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1898" s="1"/>
+    </row>
+    <row r="1899" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1899" s="1"/>
+    </row>
+    <row r="1900" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1900" s="1"/>
+    </row>
+    <row r="1901" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1901" s="1"/>
+    </row>
+    <row r="1902" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1902" s="1"/>
+    </row>
+    <row r="1903" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1903" s="1"/>
+    </row>
+    <row r="1904" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1904" s="1"/>
+    </row>
+    <row r="1905" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1905" s="1"/>
+    </row>
+    <row r="1906" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1906" s="1"/>
+    </row>
+    <row r="1907" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1907" s="1"/>
+    </row>
+    <row r="1908" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1908" s="1"/>
+    </row>
+    <row r="1909" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1909" s="1"/>
+    </row>
+    <row r="1910" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1910" s="1"/>
+    </row>
+    <row r="1911" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1911" s="1"/>
+    </row>
+    <row r="1912" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1912" s="1"/>
+    </row>
+    <row r="1913" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1913" s="1"/>
+    </row>
+    <row r="1914" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1914" s="1"/>
+    </row>
+    <row r="1915" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1915" s="1"/>
+    </row>
+    <row r="1916" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1916" s="1"/>
+    </row>
+    <row r="1917" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1917" s="1"/>
+    </row>
+    <row r="1918" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1918" s="1"/>
+    </row>
+    <row r="1919" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1919" s="1"/>
+    </row>
+    <row r="1920" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1920" s="1"/>
+    </row>
+    <row r="1921" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1921" s="1"/>
+    </row>
+    <row r="1922" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1922" s="1"/>
+    </row>
+    <row r="1923" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1923" s="1"/>
+    </row>
+    <row r="1924" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1924" s="1"/>
+    </row>
+    <row r="1925" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1925" s="1"/>
+    </row>
+    <row r="1926" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1926" s="1"/>
+    </row>
+    <row r="1927" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1927" s="1"/>
+    </row>
+    <row r="1928" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1928" s="1"/>
+    </row>
+    <row r="1929" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1929" s="1"/>
+    </row>
+    <row r="1930" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1930" s="1"/>
+    </row>
+    <row r="1931" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1931" s="1"/>
+    </row>
+    <row r="1932" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1932" s="1"/>
+    </row>
+    <row r="1933" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1933" s="3"/>
+    </row>
+    <row r="1934" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1934" s="1"/>
+    </row>
+    <row r="1935" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1935" s="1"/>
+    </row>
+    <row r="1936" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1936" s="1"/>
+    </row>
+    <row r="1937" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1937" s="1"/>
+    </row>
+    <row r="1938" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1938" s="1"/>
+    </row>
+    <row r="1939" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1939" s="1"/>
+    </row>
+    <row r="1940" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1940" s="1"/>
+    </row>
+    <row r="1941" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1941" s="1"/>
+    </row>
+    <row r="1942" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1942" s="1"/>
+    </row>
+    <row r="1943" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1943" s="1"/>
+    </row>
+    <row r="1944" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1944" s="1"/>
+    </row>
+    <row r="1945" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1945" s="1"/>
+    </row>
+    <row r="1946" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1946" s="1"/>
+    </row>
+    <row r="1947" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1947" s="1"/>
+    </row>
+    <row r="1948" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1948" s="1"/>
+    </row>
+    <row r="1949" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1949" s="1"/>
+    </row>
+    <row r="1950" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1950" s="1"/>
+    </row>
+    <row r="1951" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1951" s="1"/>
+    </row>
+    <row r="1952" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1952" s="1"/>
+    </row>
+    <row r="1953" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1953" s="1"/>
+    </row>
+    <row r="1954" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1954" s="1"/>
+    </row>
+    <row r="1955" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1955" s="1"/>
+    </row>
+    <row r="1956" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1956" s="1"/>
+    </row>
+    <row r="1957" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1957" s="1"/>
+    </row>
+    <row r="1958" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1958" s="1"/>
+    </row>
+    <row r="1959" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1959" s="1"/>
+    </row>
+    <row r="1960" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1960" s="1"/>
+    </row>
+    <row r="1961" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1961" s="1"/>
+    </row>
+    <row r="1962" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1962" s="1"/>
+    </row>
+    <row r="1963" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1963" s="1"/>
+    </row>
+    <row r="1964" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1964" s="1"/>
+    </row>
+    <row r="1965" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1965" s="1"/>
+    </row>
+    <row r="1966" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1966" s="1"/>
+    </row>
+    <row r="1967" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1967" s="1"/>
+    </row>
+    <row r="1968" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1968" s="1"/>
+    </row>
+    <row r="1969" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1969" s="1"/>
+    </row>
+    <row r="1970" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1970" s="1"/>
+    </row>
+    <row r="1971" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1971" s="1"/>
+    </row>
+    <row r="1972" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1972" s="1"/>
+    </row>
+    <row r="1973" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1973" s="1"/>
+    </row>
+    <row r="1974" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1974" s="1"/>
+    </row>
+    <row r="1975" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1975" s="1"/>
+    </row>
+    <row r="1976" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1976" s="1"/>
+    </row>
+    <row r="1977" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1977" s="1"/>
+    </row>
+    <row r="1978" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1978" s="1"/>
+    </row>
+    <row r="1979" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1979" s="1"/>
+    </row>
+    <row r="1980" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1980" s="1"/>
+    </row>
+    <row r="1981" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1981" s="1"/>
+    </row>
+    <row r="1982" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1982" s="1"/>
+    </row>
+    <row r="1983" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1983" s="1"/>
+    </row>
+    <row r="1984" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1984" s="1"/>
+    </row>
+    <row r="1985" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1985" s="1"/>
+    </row>
+    <row r="1986" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1986" s="1"/>
+    </row>
+    <row r="1987" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1987" s="1"/>
+    </row>
+    <row r="1988" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1988" s="1"/>
+    </row>
+    <row r="1989" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1989" s="1"/>
+    </row>
+    <row r="1990" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1990" s="1"/>
+    </row>
+    <row r="1991" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1991" s="1"/>
+    </row>
+    <row r="1992" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1992" s="1"/>
+    </row>
+    <row r="1993" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1993" s="1"/>
+    </row>
+    <row r="1994" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1994" s="1"/>
+    </row>
+    <row r="1995" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1995" s="1"/>
+    </row>
+    <row r="1996" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1996" s="1"/>
+    </row>
+    <row r="1997" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1997" s="1"/>
+    </row>
+    <row r="1998" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1998" s="1"/>
+    </row>
+    <row r="1999" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1999" s="1"/>
+    </row>
+    <row r="2000" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2000" s="1"/>
+    </row>
+    <row r="2001" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2001" s="1"/>
+    </row>
+    <row r="2002" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2002" s="1"/>
+    </row>
+    <row r="2003" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2003" s="1"/>
+    </row>
+    <row r="2004" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2004" s="1"/>
+    </row>
+    <row r="2005" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2005" s="1"/>
+    </row>
+    <row r="2006" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2006" s="1"/>
+    </row>
+    <row r="2007" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2007" s="1"/>
+    </row>
+    <row r="2008" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2008" s="1"/>
+    </row>
+    <row r="2009" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2009" s="1"/>
+    </row>
+    <row r="2010" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2010" s="1"/>
+    </row>
+    <row r="2011" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2011" s="1"/>
+    </row>
+    <row r="2012" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2012" s="1"/>
+    </row>
+    <row r="2013" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2013" s="1"/>
+    </row>
+    <row r="2014" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2014" s="1"/>
+    </row>
+    <row r="2015" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2015" s="1"/>
+    </row>
+    <row r="2016" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2016" s="1"/>
+    </row>
+    <row r="2017" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2017" s="1"/>
+    </row>
+    <row r="2018" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2018" s="1"/>
+    </row>
+    <row r="2019" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2019" s="1"/>
+    </row>
+    <row r="2020" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2020" s="1"/>
+    </row>
+    <row r="2021" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2021" s="1"/>
+    </row>
+    <row r="2022" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2022" s="1"/>
+    </row>
+    <row r="2023" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2023" s="1"/>
+    </row>
+    <row r="2024" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2024" s="1"/>
+    </row>
+    <row r="2025" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2025" s="1"/>
+    </row>
+    <row r="2026" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2026" s="1"/>
+    </row>
+    <row r="2027" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2027" s="1"/>
+    </row>
+    <row r="2028" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2028" s="1"/>
+    </row>
+    <row r="2029" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2029" s="1"/>
+    </row>
+    <row r="2030" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2030" s="1"/>
+    </row>
+    <row r="2031" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2031" s="1"/>
+    </row>
+    <row r="2032" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2032" s="1"/>
+    </row>
+    <row r="2033" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2033" s="1"/>
+    </row>
+    <row r="2034" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2034" s="1"/>
+    </row>
+    <row r="2035" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2035" s="1"/>
+    </row>
+    <row r="2036" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2036" s="1"/>
+    </row>
+    <row r="2037" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2037" s="1"/>
+    </row>
+    <row r="2038" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2038" s="1"/>
+    </row>
+    <row r="2039" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2039" s="1"/>
+    </row>
+    <row r="2040" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2040" s="1"/>
+    </row>
+    <row r="2041" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2041" s="1"/>
+    </row>
+    <row r="2042" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2042" s="1"/>
+    </row>
+    <row r="2043" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2043" s="1"/>
+    </row>
+    <row r="2044" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2044" s="1"/>
+    </row>
+    <row r="2045" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2045" s="1"/>
+    </row>
+    <row r="2046" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2046" s="1"/>
+    </row>
+    <row r="2047" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2047" s="1"/>
+    </row>
+    <row r="2048" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2048" s="1"/>
+    </row>
+    <row r="2049" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2049" s="1"/>
+    </row>
+    <row r="2050" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2050" s="1"/>
+    </row>
+    <row r="2051" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2051" s="1"/>
+    </row>
+    <row r="2052" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2052" s="1"/>
+    </row>
+    <row r="2053" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2053" s="1"/>
+    </row>
+    <row r="2054" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2054" s="1"/>
+    </row>
+    <row r="2055" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2055" s="1"/>
+    </row>
+    <row r="2056" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2056" s="1"/>
+    </row>
+    <row r="2057" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2057" s="1"/>
+    </row>
+    <row r="2058" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2058" s="1"/>
+    </row>
+    <row r="2059" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2059" s="1"/>
+    </row>
+    <row r="2060" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2060" s="1"/>
+    </row>
+    <row r="2061" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2061" s="1"/>
+    </row>
+    <row r="2062" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2062" s="1"/>
+    </row>
+    <row r="2063" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2063" s="1"/>
+    </row>
+    <row r="2064" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2064" s="1"/>
+    </row>
+    <row r="2065" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2065" s="1"/>
+    </row>
+    <row r="2066" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2066" s="1"/>
+    </row>
+    <row r="2067" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2067" s="1"/>
+    </row>
+    <row r="2068" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2068" s="1"/>
+    </row>
+    <row r="2069" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2069" s="1"/>
+    </row>
+    <row r="2070" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2070" s="1"/>
+    </row>
+    <row r="2071" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2071" s="1"/>
+    </row>
+    <row r="2072" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2072" s="1"/>
+    </row>
+    <row r="2073" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2073" s="1"/>
+    </row>
+    <row r="2074" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2074" s="1"/>
+    </row>
+    <row r="2075" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2075" s="1"/>
+    </row>
+    <row r="2076" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2076" s="1"/>
+    </row>
+    <row r="2077" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2077" s="1"/>
+    </row>
+    <row r="2078" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2078" s="1"/>
+    </row>
+    <row r="2079" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2079" s="1"/>
+    </row>
+    <row r="2080" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2080" s="1"/>
+    </row>
+    <row r="2081" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2081" s="1"/>
+    </row>
+    <row r="2082" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2082" s="1"/>
+    </row>
+    <row r="2083" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2083" s="1"/>
+    </row>
+    <row r="2084" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2084" s="1"/>
+    </row>
+    <row r="2085" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2085" s="1"/>
+    </row>
+    <row r="2086" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2086" s="1"/>
+    </row>
+    <row r="2087" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2087" s="1"/>
+    </row>
+    <row r="2088" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2088" s="1"/>
+    </row>
+    <row r="2089" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2089" s="1"/>
+    </row>
+    <row r="2090" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2090" s="3"/>
+    </row>
+    <row r="2091" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2091" s="1"/>
+    </row>
+    <row r="2092" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2092" s="1"/>
+    </row>
+    <row r="2093" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2093" s="1"/>
+    </row>
+    <row r="2094" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2094" s="1"/>
+    </row>
+    <row r="2095" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2095" s="1"/>
+    </row>
+    <row r="2096" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2096" s="1"/>
+    </row>
+    <row r="2097" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2097" s="1"/>
+    </row>
+    <row r="2098" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2098" s="1"/>
+    </row>
+    <row r="2099" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2099" s="1"/>
+    </row>
+    <row r="2100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2100" s="1"/>
+    </row>
+    <row r="2101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2101" s="1"/>
+    </row>
+    <row r="2102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2102" s="1"/>
+    </row>
+    <row r="2103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2103" s="1"/>
+    </row>
+    <row r="2104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2104" s="1"/>
+    </row>
+    <row r="2105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2105" s="1"/>
+    </row>
+    <row r="2106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2106" s="1"/>
+    </row>
+    <row r="2107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2107" s="1"/>
+    </row>
+    <row r="2108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2108" s="1"/>
+    </row>
+    <row r="2109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2109" s="1"/>
+    </row>
+    <row r="2110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2110" s="1"/>
+    </row>
+    <row r="2111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2111" s="1"/>
+    </row>
+    <row r="2112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2112" s="1"/>
+    </row>
+    <row r="2113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2113" s="1"/>
+    </row>
+    <row r="2114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2114" s="1"/>
+    </row>
+    <row r="2115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2115" s="1"/>
+    </row>
+    <row r="2116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2116" s="1"/>
+    </row>
+    <row r="2117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2117" s="1"/>
+    </row>
+    <row r="2118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2118" s="1"/>
+    </row>
+    <row r="2119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2119" s="1"/>
+    </row>
+    <row r="2120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2120" s="1"/>
+    </row>
+    <row r="2121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2121" s="1"/>
+    </row>
+    <row r="2122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2122" s="1"/>
+    </row>
+    <row r="2123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2123" s="1"/>
+    </row>
+    <row r="2124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2124" s="1"/>
+    </row>
+    <row r="2125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2125" s="1"/>
+    </row>
+    <row r="2126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2126" s="1"/>
+    </row>
+    <row r="2127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2127" s="1"/>
+    </row>
+    <row r="2128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2128" s="1"/>
+    </row>
+    <row r="2129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2129" s="1"/>
+    </row>
+    <row r="2130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2130" s="1"/>
+    </row>
+    <row r="2131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2131" s="1"/>
+    </row>
+    <row r="2132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2132" s="1"/>
+    </row>
+    <row r="2133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2133" s="1"/>
+    </row>
+    <row r="2134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2134" s="1"/>
+    </row>
+    <row r="2135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2135" s="1"/>
+    </row>
+    <row r="2136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2136" s="1"/>
+    </row>
+    <row r="2137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2137" s="1"/>
+    </row>
+    <row r="2138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2138" s="1"/>
+    </row>
+    <row r="2139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2139" s="1"/>
+    </row>
+    <row r="2140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2140" s="1"/>
+    </row>
+    <row r="2141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2141" s="1"/>
+    </row>
+    <row r="2142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2142" s="1"/>
+    </row>
+    <row r="2143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2143" s="1"/>
+    </row>
+    <row r="2144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2144" s="1"/>
+    </row>
+    <row r="2145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2145" s="1"/>
+    </row>
+    <row r="2146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2146" s="1"/>
+    </row>
+    <row r="2147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2147" s="1"/>
+    </row>
+    <row r="2148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2148" s="1"/>
+    </row>
+    <row r="2149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2149" s="1"/>
+    </row>
+    <row r="2150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2150" s="1"/>
+    </row>
+    <row r="2151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2151" s="1"/>
+    </row>
+    <row r="2152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2152" s="1"/>
+    </row>
+    <row r="2153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2153" s="1"/>
+    </row>
+    <row r="2154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2154" s="1"/>
+    </row>
+    <row r="2155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2155" s="1"/>
+    </row>
+    <row r="2156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2156" s="1"/>
+    </row>
+    <row r="2157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2157" s="1"/>
+    </row>
+    <row r="2158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2158" s="1"/>
+    </row>
+    <row r="2159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2159" s="1"/>
+    </row>
+    <row r="2160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2160" s="1"/>
+    </row>
+    <row r="2161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2161" s="1"/>
+    </row>
+    <row r="2162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2162" s="1"/>
+    </row>
+    <row r="2163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2163" s="1"/>
+    </row>
+    <row r="2164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2164" s="1"/>
+    </row>
+    <row r="2165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2165" s="1"/>
+    </row>
+    <row r="2166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2166" s="1"/>
+    </row>
+    <row r="2167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2167" s="1"/>
+    </row>
+    <row r="2168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2168" s="1"/>
+    </row>
+    <row r="2169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2169" s="1"/>
+    </row>
+    <row r="2170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2170" s="1"/>
+    </row>
+    <row r="2171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2171" s="1"/>
+    </row>
+    <row r="2172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2172" s="1"/>
+    </row>
+    <row r="2173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2173" s="1"/>
+    </row>
+    <row r="2174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2174" s="1"/>
+    </row>
+    <row r="2175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2175" s="1"/>
+    </row>
+    <row r="2176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2176" s="1"/>
+    </row>
+    <row r="2177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2177" s="1"/>
+    </row>
+    <row r="2178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2178" s="1"/>
+    </row>
+    <row r="2179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2179" s="1"/>
+    </row>
+    <row r="2180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2180" s="1"/>
+    </row>
+    <row r="2181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2181" s="1"/>
+    </row>
+    <row r="2182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2182" s="1"/>
+    </row>
+    <row r="2183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2183" s="1"/>
+    </row>
+    <row r="2184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2184" s="1"/>
+    </row>
+    <row r="2185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2185" s="1"/>
+    </row>
+    <row r="2186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2186" s="1"/>
+    </row>
+    <row r="2187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2187" s="1"/>
+    </row>
+    <row r="2188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2188" s="1"/>
+    </row>
+    <row r="2189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2189" s="1"/>
+    </row>
+    <row r="2190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2190" s="1"/>
+    </row>
+    <row r="2191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2191" s="1"/>
+    </row>
+    <row r="2192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2192" s="1"/>
+    </row>
+    <row r="2193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2193" s="1"/>
+    </row>
+    <row r="2194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2194" s="1"/>
+    </row>
+    <row r="2195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2195" s="1"/>
+    </row>
+    <row r="2196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2196" s="1"/>
+    </row>
+    <row r="2197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2197" s="1"/>
+    </row>
+    <row r="2198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2198" s="1"/>
+    </row>
+    <row r="2199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2199" s="1"/>
+    </row>
+    <row r="2200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2200" s="1"/>
+    </row>
+    <row r="2201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2201" s="1"/>
+    </row>
+    <row r="2202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2202" s="1"/>
+    </row>
+    <row r="2203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2203" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:F885">
-    <sortCondition ref="A1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>